<commit_message>
Sprint 2 Update Dhruv
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9936BCFA-3ED7-492A-941E-AE718BA248C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2763B85-D85B-4285-8D20-DF1A0BE36589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="254">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -831,6 +831,12 @@
   </si>
   <si>
     <t>Less communication</t>
+  </si>
+  <si>
+    <t>Fewer than 15 sibiling</t>
+  </si>
+  <si>
+    <t>List large age difference</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1079,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1153,6 +1159,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2493,7 +2500,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2808,6 +2815,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>3</v>
+      </c>
       <c r="B20" s="27" t="s">
         <v>128</v>
       </c>
@@ -2818,7 +2828,7 @@
         <v>195</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2835,7 +2845,7 @@
         <v>195</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2866,10 +2876,13 @@
         <v>195</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>3</v>
+      </c>
       <c r="B24" s="27" t="s">
         <v>147</v>
       </c>
@@ -2880,7 +2893,7 @@
         <v>195</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3595,7 +3608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -4093,7 +4106,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4233,7 +4246,7 @@
         <v>195</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E6" s="12">
         <v>60</v>
@@ -4241,9 +4254,15 @@
       <c r="F6" s="12">
         <v>100</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="G6" s="12">
+        <v>15</v>
+      </c>
+      <c r="H6" s="12">
+        <v>20</v>
+      </c>
+      <c r="I6" s="51">
+        <v>44469</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -4256,7 +4275,7 @@
         <v>195</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E7" s="12">
         <v>60</v>
@@ -4264,9 +4283,15 @@
       <c r="F7" s="12">
         <v>100</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="12">
+        <v>48</v>
+      </c>
+      <c r="H7" s="12">
+        <v>40</v>
+      </c>
+      <c r="I7" s="51">
+        <v>44469</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -4417,11 +4442,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
@@ -4453,23 +4481,47 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="A2" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="12">
+        <v>30</v>
+      </c>
+      <c r="F2" s="12">
+        <v>60</v>
+      </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="A3" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" s="12">
+        <v>30</v>
+      </c>
+      <c r="F3" s="12">
+        <v>60</v>
+      </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -4598,8 +4650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added US32 and Completed Sprint 2
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dishantnaik/Documents/MS/Semester_3/SSW 555/Project/CS_555_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2763B85-D85B-4285-8D20-DF1A0BE36589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2987800A-4EF4-D049-8C5C-787222E2EFC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14460" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="254">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1079,7 +1079,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1153,13 +1153,14 @@
     <xf numFmtId="49" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1274,7 +1275,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1345,7 +1346,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2335,16 +2336,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.90625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="12" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="12" customWidth="1"/>
+    <col min="4" max="5" width="20.5" style="12" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
@@ -2361,7 +2362,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="21" t="s">
         <v>192</v>
       </c>
@@ -2378,7 +2379,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
         <v>193</v>
       </c>
@@ -2395,7 +2396,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="25" t="s">
         <v>194</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="27" t="s">
         <v>195</v>
       </c>
@@ -2429,7 +2430,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="34" t="s">
         <v>201</v>
       </c>
@@ -2446,7 +2447,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="38" t="s">
         <v>215</v>
       </c>
@@ -2463,16 +2464,16 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="D9" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="51"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
@@ -2499,20 +2500,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="6.6328125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
@@ -2529,7 +2530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2546,7 +2547,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -2563,7 +2564,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" s="21" t="s">
         <v>141</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -2594,7 +2595,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" s="21" t="s">
         <v>146</v>
       </c>
@@ -2608,7 +2609,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -2625,7 +2626,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>2</v>
       </c>
@@ -2642,7 +2643,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" s="21" t="s">
         <v>151</v>
       </c>
@@ -2656,7 +2657,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>2</v>
       </c>
@@ -2673,7 +2674,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>2</v>
       </c>
@@ -2690,7 +2691,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" s="23" t="s">
         <v>116</v>
       </c>
@@ -2704,7 +2705,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B13" s="23" t="s">
         <v>119</v>
       </c>
@@ -2718,7 +2719,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" s="23" t="s">
         <v>120</v>
       </c>
@@ -2732,7 +2733,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="12">
         <v>1</v>
       </c>
@@ -2749,7 +2750,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="12">
         <v>1</v>
       </c>
@@ -2766,7 +2767,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" s="23" t="s">
         <v>138</v>
       </c>
@@ -2780,7 +2781,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="12">
         <v>1</v>
       </c>
@@ -2797,7 +2798,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="12">
         <v>1</v>
       </c>
@@ -2814,7 +2815,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="12">
         <v>3</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="12">
         <v>2</v>
       </c>
@@ -2848,7 +2849,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B22" s="27" t="s">
         <v>136</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="12">
         <v>2</v>
       </c>
@@ -2879,7 +2880,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="12">
         <v>3</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B25" s="27" t="s">
         <v>153</v>
       </c>
@@ -2910,7 +2911,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B26" s="25" t="s">
         <v>121</v>
       </c>
@@ -2924,9 +2925,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>122</v>
@@ -2941,7 +2942,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="12">
         <v>1</v>
       </c>
@@ -2958,7 +2959,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="12">
+        <v>3</v>
+      </c>
       <c r="B29" s="25" t="s">
         <v>127</v>
       </c>
@@ -2969,10 +2973,10 @@
         <v>194</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="12">
         <v>2</v>
       </c>
@@ -2989,7 +2993,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" s="12">
+        <v>2</v>
+      </c>
       <c r="B31" s="25" t="s">
         <v>145</v>
       </c>
@@ -3000,10 +3007,10 @@
         <v>194</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -3020,7 +3027,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B33" s="25" t="s">
         <v>155</v>
       </c>
@@ -3034,7 +3041,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B34" s="34" t="s">
         <v>124</v>
       </c>
@@ -3048,7 +3055,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B35" s="34" t="s">
         <v>125</v>
       </c>
@@ -3062,7 +3069,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -3079,7 +3086,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="12">
         <v>2</v>
       </c>
@@ -3096,7 +3103,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="12">
         <v>2</v>
       </c>
@@ -3113,7 +3120,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="12">
         <v>1</v>
       </c>
@@ -3130,7 +3137,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="12">
         <v>1</v>
       </c>
@@ -3147,7 +3154,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B41" s="34" t="s">
         <v>208</v>
       </c>
@@ -3161,7 +3168,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="12">
         <v>2</v>
       </c>
@@ -3178,7 +3185,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B43" s="38" t="s">
         <v>137</v>
       </c>
@@ -3192,7 +3199,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B44" s="38" t="s">
         <v>139</v>
       </c>
@@ -3206,7 +3213,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B45" s="38" t="s">
         <v>150</v>
       </c>
@@ -3220,7 +3227,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B46" s="38" t="s">
         <v>154</v>
       </c>
@@ -3234,7 +3241,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="12">
         <v>1</v>
       </c>
@@ -3251,7 +3258,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="12">
         <v>2</v>
       </c>
@@ -3268,7 +3275,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="12">
         <v>1</v>
       </c>
@@ -3285,7 +3292,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B50" s="39"/>
     </row>
   </sheetData>
@@ -3308,47 +3315,47 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="5"/>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3371,7 +3378,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3387,7 +3394,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3412,7 +3419,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>164</v>
       </c>
@@ -3437,7 +3444,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>165</v>
       </c>
@@ -3462,7 +3469,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>166</v>
       </c>
@@ -3498,20 +3505,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="2"/>
-    <col min="2" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3531,7 +3538,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="16">
         <v>42633</v>
       </c>
@@ -3545,7 +3552,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="16">
         <v>42657</v>
       </c>
@@ -3566,7 +3573,7 @@
         <v>30.054446460980031</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="16">
         <v>42683</v>
       </c>
@@ -3576,7 +3583,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="16">
         <v>42708</v>
       </c>
@@ -3586,7 +3593,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="16">
         <v>42728</v>
       </c>
@@ -3612,21 +3619,21 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="11" style="12"/>
-    <col min="5" max="5" width="6.90625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="6.6328125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="12" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -3655,7 +3662,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>142</v>
       </c>
@@ -3684,7 +3691,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>143</v>
       </c>
@@ -3713,7 +3720,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>144</v>
       </c>
@@ -3742,7 +3749,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>130</v>
       </c>
@@ -3771,7 +3778,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>134</v>
       </c>
@@ -3800,7 +3807,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>123</v>
       </c>
@@ -3829,7 +3836,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>152</v>
       </c>
@@ -3858,7 +3865,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>117</v>
       </c>
@@ -3887,7 +3894,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>118</v>
       </c>
@@ -3916,7 +3923,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>206</v>
       </c>
@@ -3945,7 +3952,7 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>207</v>
       </c>
@@ -3974,7 +3981,7 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>126</v>
       </c>
@@ -4003,7 +4010,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>220</v>
       </c>
@@ -4032,7 +4039,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
         <v>222</v>
       </c>
@@ -4061,35 +4068,35 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="13" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="13" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="13" t="s">
         <v>251</v>
       </c>
@@ -4106,15 +4113,15 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -4143,7 +4150,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>148</v>
       </c>
@@ -4166,7 +4173,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>149</v>
       </c>
@@ -4189,18 +4196,18 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>194</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E4" s="12">
         <v>60</v>
@@ -4208,11 +4215,17 @@
       <c r="F4" s="12">
         <v>90</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G4" s="12">
+        <v>25</v>
+      </c>
+      <c r="H4" s="12">
+        <v>25</v>
+      </c>
+      <c r="I4" s="52">
+        <v>42668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>135</v>
       </c>
@@ -4223,7 +4236,7 @@
         <v>194</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E5" s="12">
         <v>40</v>
@@ -4231,11 +4244,17 @@
       <c r="F5" s="12">
         <v>90</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G5" s="12">
+        <v>20</v>
+      </c>
+      <c r="H5" s="12">
+        <v>15</v>
+      </c>
+      <c r="I5" s="52">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>140</v>
       </c>
@@ -4260,11 +4279,11 @@
       <c r="H6" s="12">
         <v>20</v>
       </c>
-      <c r="I6" s="51">
+      <c r="I6" s="49">
         <v>44469</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>129</v>
       </c>
@@ -4289,11 +4308,11 @@
       <c r="H7" s="12">
         <v>40</v>
       </c>
-      <c r="I7" s="51">
+      <c r="I7" s="49">
         <v>44469</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>114</v>
       </c>
@@ -4316,7 +4335,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>115</v>
       </c>
@@ -4339,7 +4358,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>133</v>
       </c>
@@ -4362,7 +4381,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>221</v>
       </c>
@@ -4385,7 +4404,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>131</v>
       </c>
@@ -4408,7 +4427,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>132</v>
       </c>
@@ -4442,16 +4461,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4480,7 +4499,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>128</v>
       </c>
@@ -4503,7 +4522,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>147</v>
       </c>
@@ -4526,29 +4545,53 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4" s="12">
+        <v>120</v>
+      </c>
+      <c r="F4" s="12">
+        <v>120</v>
+      </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5" s="12">
+        <v>60</v>
+      </c>
+      <c r="F5" s="12">
+        <v>60</v>
+      </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -4559,7 +4602,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -4570,7 +4613,7 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -4581,7 +4624,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -4606,12 +4649,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4650,17 +4693,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>113</v>
       </c>
@@ -4671,7 +4714,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="23" t="s">
         <v>114</v>
       </c>
@@ -4682,7 +4725,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
         <v>115</v>
       </c>
@@ -4693,7 +4736,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
         <v>116</v>
       </c>
@@ -4704,7 +4747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" s="27" t="s">
         <v>117</v>
       </c>
@@ -4715,7 +4758,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" s="27" t="s">
         <v>118</v>
       </c>
@@ -4726,7 +4769,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="23" t="s">
         <v>119</v>
       </c>
@@ -4737,7 +4780,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="31" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="31" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" s="23" t="s">
         <v>120</v>
       </c>
@@ -4748,7 +4791,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" s="25" t="s">
         <v>121</v>
       </c>
@@ -4759,7 +4802,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="25" t="s">
         <v>122</v>
       </c>
@@ -4770,7 +4813,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
         <v>123</v>
       </c>
@@ -4781,7 +4824,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="34" t="s">
         <v>124</v>
       </c>
@@ -4792,7 +4835,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" s="34" t="s">
         <v>125</v>
       </c>
@@ -4803,7 +4846,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="36" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="36" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" s="34" t="s">
         <v>126</v>
       </c>
@@ -4814,7 +4857,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
         <v>127</v>
       </c>
@@ -4825,7 +4868,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="27" t="s">
         <v>128</v>
       </c>
@@ -4836,7 +4879,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="27" t="s">
         <v>129</v>
       </c>
@@ -4847,7 +4890,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" s="23" t="s">
         <v>130</v>
       </c>
@@ -4858,7 +4901,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="34" t="s">
         <v>131</v>
       </c>
@@ -4869,7 +4912,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="34" t="s">
         <v>132</v>
       </c>
@@ -4880,7 +4923,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="38" t="s">
         <v>133</v>
       </c>
@@ -4891,7 +4934,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="23" t="s">
         <v>134</v>
       </c>
@@ -4902,7 +4945,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" s="25" t="s">
         <v>135</v>
       </c>
@@ -4913,7 +4956,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" s="27" t="s">
         <v>136</v>
       </c>
@@ -4924,7 +4967,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="37" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="37" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="38" t="s">
         <v>137</v>
       </c>
@@ -4935,7 +4978,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="23" t="s">
         <v>138</v>
       </c>
@@ -4946,7 +4989,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="37" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="37" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A27" s="38" t="s">
         <v>139</v>
       </c>
@@ -4957,7 +5000,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="27" t="s">
         <v>140</v>
       </c>
@@ -4968,7 +5011,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" s="21" t="s">
         <v>141</v>
       </c>
@@ -4979,7 +5022,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="21" t="s">
         <v>142</v>
       </c>
@@ -4990,7 +5033,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="21" t="s">
         <v>143</v>
       </c>
@@ -5001,7 +5044,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="21" t="s">
         <v>144</v>
       </c>
@@ -5012,7 +5055,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="25" t="s">
         <v>145</v>
       </c>
@@ -5023,7 +5066,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" s="21" t="s">
         <v>146</v>
       </c>
@@ -5034,7 +5077,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" s="27" t="s">
         <v>147</v>
       </c>
@@ -5045,7 +5088,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" s="21" t="s">
         <v>148</v>
       </c>
@@ -5056,7 +5099,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" s="21" t="s">
         <v>149</v>
       </c>
@@ -5067,7 +5110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="37" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" s="38" t="s">
         <v>150</v>
       </c>
@@ -5078,7 +5121,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" s="21" t="s">
         <v>151</v>
       </c>
@@ -5089,7 +5132,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" s="25" t="s">
         <v>152</v>
       </c>
@@ -5100,7 +5143,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" s="27" t="s">
         <v>153</v>
       </c>
@@ -5111,7 +5154,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" s="38" t="s">
         <v>154</v>
       </c>
@@ -5122,7 +5165,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" s="25" t="s">
         <v>155</v>
       </c>
@@ -5133,7 +5176,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A44" s="34" t="s">
         <v>206</v>
       </c>
@@ -5144,7 +5187,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A45" s="34" t="s">
         <v>207</v>
       </c>
@@ -5155,7 +5198,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A46" s="34" t="s">
         <v>208</v>
       </c>
@@ -5166,7 +5209,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="38" t="s">
         <v>220</v>
       </c>
@@ -5177,7 +5220,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="37" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" s="38" t="s">
         <v>221</v>
       </c>
@@ -5188,7 +5231,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="38" t="s">
         <v>222</v>
       </c>

</xml_diff>

<commit_message>
Completed sprint 2 and planned sprint 3 stories and also updated backlog.
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dishantnaik/Documents/MS/Semester_3/SSW 555/Project/CS_555_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2987800A-4EF4-D049-8C5C-787222E2EFC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23FDF78-224D-4346-8CDD-AA39B31592F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14460" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="255">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -837,6 +837,9 @@
   </si>
   <si>
     <t>List large age difference</t>
+  </si>
+  <si>
+    <t>Refactoring Week</t>
   </si>
 </sst>
 </file>
@@ -1154,13 +1157,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1275,7 +1278,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1346,7 +1349,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1410,23 +1413,29 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
+              <c:f>Burndown!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>m/d</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>42633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42657</c:v>
+                  <c:v>42647</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>42654</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42668</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>42683</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>42708</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>42728</c:v>
                 </c:pt>
               </c:numCache>
@@ -1434,15 +1443,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$7</c:f>
+              <c:f>Burndown!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1975,13 +1990,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>948267</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>160867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>397934</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>25401</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2336,16 +2351,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="12" customWidth="1"/>
     <col min="4" max="5" width="20.5" style="12" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
@@ -2362,7 +2377,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>192</v>
       </c>
@@ -2379,7 +2394,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>193</v>
       </c>
@@ -2396,7 +2411,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>194</v>
       </c>
@@ -2413,7 +2428,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>195</v>
       </c>
@@ -2430,7 +2445,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
         <v>201</v>
       </c>
@@ -2447,7 +2462,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>215</v>
       </c>
@@ -2464,16 +2479,16 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D9" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
@@ -2500,20 +2515,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="6.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
@@ -2530,7 +2545,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2547,7 +2562,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -2564,7 +2579,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
         <v>141</v>
       </c>
@@ -2578,7 +2593,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -2595,7 +2610,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
       <c r="B6" s="21" t="s">
         <v>146</v>
       </c>
@@ -2606,10 +2624,10 @@
         <v>192</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -2623,10 +2641,10 @@
         <v>192</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>2</v>
       </c>
@@ -2640,10 +2658,13 @@
         <v>192</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
+        <v>3</v>
+      </c>
       <c r="B9" s="21" t="s">
         <v>151</v>
       </c>
@@ -2654,10 +2675,10 @@
         <v>192</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>2</v>
       </c>
@@ -2674,7 +2695,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>2</v>
       </c>
@@ -2691,7 +2712,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
         <v>116</v>
       </c>
@@ -2705,7 +2726,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
         <v>119</v>
       </c>
@@ -2719,7 +2740,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
         <v>120</v>
       </c>
@@ -2733,7 +2754,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>1</v>
       </c>
@@ -2750,7 +2771,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <v>1</v>
       </c>
@@ -2767,7 +2788,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
         <v>138</v>
       </c>
@@ -2781,7 +2802,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>1</v>
       </c>
@@ -2798,7 +2819,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <v>1</v>
       </c>
@@ -2815,7 +2836,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <v>3</v>
       </c>
@@ -2832,7 +2853,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>2</v>
       </c>
@@ -2849,7 +2870,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="27" t="s">
         <v>136</v>
       </c>
@@ -2863,7 +2884,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>2</v>
       </c>
@@ -2880,7 +2901,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <v>3</v>
       </c>
@@ -2897,7 +2918,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" s="27" t="s">
         <v>153</v>
       </c>
@@ -2911,7 +2932,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="25" t="s">
         <v>121</v>
       </c>
@@ -2925,7 +2946,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <v>3</v>
       </c>
@@ -2942,7 +2963,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
         <v>1</v>
       </c>
@@ -2959,7 +2980,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <v>3</v>
       </c>
@@ -2976,7 +2997,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="12">
         <v>2</v>
       </c>
@@ -2993,7 +3014,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="12">
         <v>2</v>
       </c>
@@ -3010,7 +3031,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -3027,7 +3048,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" s="25" t="s">
         <v>155</v>
       </c>
@@ -3041,7 +3062,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" s="34" t="s">
         <v>124</v>
       </c>
@@ -3055,7 +3076,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" s="34" t="s">
         <v>125</v>
       </c>
@@ -3069,7 +3090,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -3086,7 +3107,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="12">
         <v>2</v>
       </c>
@@ -3103,7 +3124,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="12">
         <v>2</v>
       </c>
@@ -3120,7 +3141,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="12">
         <v>1</v>
       </c>
@@ -3137,7 +3158,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="12">
         <v>1</v>
       </c>
@@ -3154,7 +3175,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" s="34" t="s">
         <v>208</v>
       </c>
@@ -3168,7 +3189,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="12">
         <v>2</v>
       </c>
@@ -3185,7 +3206,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" s="38" t="s">
         <v>137</v>
       </c>
@@ -3199,7 +3220,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="38" t="s">
         <v>139</v>
       </c>
@@ -3213,7 +3234,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45" s="38" t="s">
         <v>150</v>
       </c>
@@ -3227,7 +3248,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B46" s="38" t="s">
         <v>154</v>
       </c>
@@ -3241,7 +3262,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="12">
         <v>1</v>
       </c>
@@ -3258,7 +3279,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="12">
         <v>2</v>
       </c>
@@ -3275,7 +3296,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="12">
         <v>1</v>
       </c>
@@ -3292,7 +3313,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B50" s="39"/>
     </row>
   </sheetData>
@@ -3315,47 +3336,47 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="5"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3378,7 +3399,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3394,7 +3415,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3419,7 +3440,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>164</v>
       </c>
@@ -3444,7 +3465,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>165</v>
       </c>
@@ -3469,7 +3490,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>166</v>
       </c>
@@ -3503,22 +3524,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3538,7 +3560,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="16">
         <v>42633</v>
       </c>
@@ -3552,9 +3574,9 @@
       <c r="E2" s="12"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
-        <v>42657</v>
+        <v>42647</v>
       </c>
       <c r="B3" s="12">
         <v>34</v>
@@ -3573,35 +3595,73 @@
         <v>30.054446460980031</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
-        <v>42683</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+        <v>42654</v>
+      </c>
+      <c r="B4" s="12">
+        <v>34</v>
+      </c>
+      <c r="C4" s="12">
+        <v>14</v>
+      </c>
+      <c r="D4" s="12">
+        <v>552</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1102</v>
+      </c>
+      <c r="F4" s="17">
+        <v>30.1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
-        <v>42708</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+        <v>42668</v>
+      </c>
+      <c r="B5" s="12">
+        <v>22</v>
+      </c>
+      <c r="C5" s="12">
+        <f>B4-B5</f>
+        <v>12</v>
+      </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
-        <v>42728</v>
+        <v>42683</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="16">
+        <v>42708</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="16">
+        <v>42728</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3619,21 +3679,21 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="12" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="12" customWidth="1"/>
     <col min="4" max="4" width="11" style="12"/>
-    <col min="5" max="5" width="6.83203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="12" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -3662,7 +3722,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>142</v>
       </c>
@@ -3691,7 +3751,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>143</v>
       </c>
@@ -3720,7 +3780,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>144</v>
       </c>
@@ -3749,7 +3809,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>130</v>
       </c>
@@ -3778,7 +3838,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>134</v>
       </c>
@@ -3807,7 +3867,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>123</v>
       </c>
@@ -3836,7 +3896,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>152</v>
       </c>
@@ -3865,7 +3925,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>117</v>
       </c>
@@ -3894,7 +3954,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>118</v>
       </c>
@@ -3923,7 +3983,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>206</v>
       </c>
@@ -3952,7 +4012,7 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>207</v>
       </c>
@@ -3981,7 +4041,7 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>126</v>
       </c>
@@ -4010,7 +4070,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>220</v>
       </c>
@@ -4039,7 +4099,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>222</v>
       </c>
@@ -4068,35 +4128,35 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="13" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="13" t="s">
         <v>251</v>
       </c>
@@ -4113,15 +4173,15 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -4150,7 +4210,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>148</v>
       </c>
@@ -4161,7 +4221,7 @@
         <v>192</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E2" s="12">
         <v>25</v>
@@ -4169,11 +4229,17 @@
       <c r="F2" s="12">
         <v>60</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G2" s="12">
+        <v>15</v>
+      </c>
+      <c r="H2" s="12">
+        <v>30</v>
+      </c>
+      <c r="I2" s="50">
+        <v>42668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>149</v>
       </c>
@@ -4184,7 +4250,7 @@
         <v>192</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E3" s="12">
         <v>25</v>
@@ -4192,11 +4258,17 @@
       <c r="F3" s="12">
         <v>60</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G3" s="12">
+        <v>15</v>
+      </c>
+      <c r="H3" s="12">
+        <v>30</v>
+      </c>
+      <c r="I3" s="50">
+        <v>42668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>145</v>
       </c>
@@ -4221,11 +4293,11 @@
       <c r="H4" s="12">
         <v>25</v>
       </c>
-      <c r="I4" s="52">
+      <c r="I4" s="50">
         <v>42668</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>135</v>
       </c>
@@ -4250,11 +4322,11 @@
       <c r="H5" s="12">
         <v>15</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="50">
         <v>42667</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>140</v>
       </c>
@@ -4283,7 +4355,7 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>129</v>
       </c>
@@ -4312,7 +4384,7 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>114</v>
       </c>
@@ -4335,7 +4407,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>115</v>
       </c>
@@ -4358,7 +4430,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>133</v>
       </c>
@@ -4381,7 +4453,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>221</v>
       </c>
@@ -4404,7 +4476,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>131</v>
       </c>
@@ -4427,7 +4499,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>132</v>
       </c>
@@ -4461,16 +4533,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4499,7 +4571,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>128</v>
       </c>
@@ -4522,7 +4594,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>147</v>
       </c>
@@ -4545,7 +4617,7 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>122</v>
       </c>
@@ -4568,7 +4640,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>127</v>
       </c>
@@ -4591,29 +4663,53 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" s="12">
+        <v>25</v>
+      </c>
+      <c r="F6" s="12">
+        <v>60</v>
+      </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" s="12">
+        <v>25</v>
+      </c>
+      <c r="F7" s="12">
+        <v>60</v>
+      </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -4624,7 +4720,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -4649,12 +4745,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4693,17 +4789,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>113</v>
       </c>
@@ -4714,7 +4810,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>114</v>
       </c>
@@ -4725,7 +4821,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>115</v>
       </c>
@@ -4736,7 +4832,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>116</v>
       </c>
@@ -4747,7 +4843,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>117</v>
       </c>
@@ -4758,7 +4854,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>118</v>
       </c>
@@ -4769,7 +4865,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>119</v>
       </c>
@@ -4780,7 +4876,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="31" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" s="31" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>120</v>
       </c>
@@ -4791,7 +4887,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>121</v>
       </c>
@@ -4802,7 +4898,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>122</v>
       </c>
@@ -4813,7 +4909,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>123</v>
       </c>
@@ -4824,7 +4920,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="34" t="s">
         <v>124</v>
       </c>
@@ -4835,7 +4931,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
         <v>125</v>
       </c>
@@ -4846,7 +4942,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="36" customFormat="1" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A14" s="34" t="s">
         <v>126</v>
       </c>
@@ -4857,7 +4953,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>127</v>
       </c>
@@ -4868,7 +4964,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>128</v>
       </c>
@@ -4879,7 +4975,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>129</v>
       </c>
@@ -4890,7 +4986,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>130</v>
       </c>
@@ -4901,7 +4997,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="34" t="s">
         <v>131</v>
       </c>
@@ -4912,7 +5008,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
         <v>132</v>
       </c>
@@ -4923,7 +5019,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="s">
         <v>133</v>
       </c>
@@ -4934,7 +5030,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>134</v>
       </c>
@@ -4945,7 +5041,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
         <v>135</v>
       </c>
@@ -4956,7 +5052,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
         <v>136</v>
       </c>
@@ -4967,7 +5063,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="37" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" s="37" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" s="38" t="s">
         <v>137</v>
       </c>
@@ -4978,7 +5074,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
         <v>138</v>
       </c>
@@ -4989,7 +5085,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="37" customFormat="1" ht="119" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" s="37" customFormat="1" ht="110.25" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
         <v>139</v>
       </c>
@@ -5000,7 +5096,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
         <v>140</v>
       </c>
@@ -5011,7 +5107,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>141</v>
       </c>
@@ -5022,7 +5118,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>142</v>
       </c>
@@ -5033,7 +5129,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
         <v>143</v>
       </c>
@@ -5044,7 +5140,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
         <v>144</v>
       </c>
@@ -5055,7 +5151,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
         <v>145</v>
       </c>
@@ -5066,7 +5162,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
         <v>146</v>
       </c>
@@ -5077,7 +5173,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="s">
         <v>147</v>
       </c>
@@ -5088,7 +5184,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>148</v>
       </c>
@@ -5099,7 +5195,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>149</v>
       </c>
@@ -5110,7 +5206,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" s="38" t="s">
         <v>150</v>
       </c>
@@ -5121,7 +5217,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>151</v>
       </c>
@@ -5132,7 +5228,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
         <v>152</v>
       </c>
@@ -5143,7 +5239,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
         <v>153</v>
       </c>
@@ -5154,7 +5250,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" s="38" t="s">
         <v>154</v>
       </c>
@@ -5165,7 +5261,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
         <v>155</v>
       </c>
@@ -5176,7 +5272,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A44" s="34" t="s">
         <v>206</v>
       </c>
@@ -5187,7 +5283,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A45" s="34" t="s">
         <v>207</v>
       </c>
@@ -5198,7 +5294,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A46" s="34" t="s">
         <v>208</v>
       </c>
@@ -5209,7 +5305,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="38" t="s">
         <v>220</v>
       </c>
@@ -5220,7 +5316,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="38" t="s">
         <v>221</v>
       </c>
@@ -5231,7 +5327,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="38" t="s">
         <v>222</v>
       </c>

</xml_diff>

<commit_message>
Added Project06#3.2 Make 2 lists: things you want to keep doing things that you want to avoid doing in the future
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23FDF78-224D-4346-8CDD-AA39B31592F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624206FD-267E-40D3-BB86-68EDD1E7F564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="268">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -840,6 +840,45 @@
   </si>
   <si>
     <t>Refactoring Week</t>
+  </si>
+  <si>
+    <t>Make 2 lists:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Reuse code </t>
+  </si>
+  <si>
+    <t>2. Refactor code after each sprint</t>
+  </si>
+  <si>
+    <t>3. Follow function naming standards</t>
+  </si>
+  <si>
+    <t>Things that want to avoid doing in the future</t>
+  </si>
+  <si>
+    <t>Things want to keep doing</t>
+  </si>
+  <si>
+    <t>4. Write valid testcases</t>
+  </si>
+  <si>
+    <t>1. Wait untill last moment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Run testcases after integrating code in each sprint </t>
+  </si>
+  <si>
+    <t>2. Avoid duplicate code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Avoid complex code </t>
+  </si>
+  <si>
+    <t>4. Avoid breaking testcases</t>
+  </si>
+  <si>
+    <t>6. Update testdata for each usecase</t>
   </si>
 </sst>
 </file>
@@ -850,7 +889,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -902,6 +941,11 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1082,7 +1126,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1164,6 +1208,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4170,10 +4218,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4521,6 +4569,66 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="53"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D21" s="54"/>
+      <c r="E21" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="54" t="s">
+        <v>256</v>
+      </c>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="54" t="s">
+        <v>257</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="54" t="s">
+        <v>258</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="54" t="s">
+        <v>261</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="54" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="54" t="s">
+        <v>267</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4533,7 +4641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating details about the next Sprint
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuragaman/Desktop/StudentID#10446036/CS_555_Project-master 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624206FD-267E-40D3-BB86-68EDD1E7F564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53958FE-419E-CD4E-8487-F03AB6B0C78D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="268">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1202,16 +1202,16 @@
     </xf>
     <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1326,7 +1326,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1397,7 +1397,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2396,19 +2396,19 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="12" customWidth="1"/>
     <col min="4" max="5" width="20.5" style="12" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="21" t="s">
         <v>192</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
         <v>193</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="25" t="s">
         <v>194</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="27" t="s">
         <v>195</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="34" t="s">
         <v>201</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="38" t="s">
         <v>215</v>
       </c>
@@ -2527,16 +2527,16 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="D9" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="54"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
@@ -2564,19 +2564,19 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:E9"/>
+      <selection activeCell="B12" sqref="B12:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="6.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" s="21" t="s">
         <v>141</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>2</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>3</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>2</v>
       </c>
@@ -2740,10 +2740,10 @@
         <v>193</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>2</v>
       </c>
@@ -2757,10 +2757,13 @@
         <v>193</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="12">
+        <v>3</v>
+      </c>
       <c r="B12" s="23" t="s">
         <v>116</v>
       </c>
@@ -2771,10 +2774,13 @@
         <v>193</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="12">
+        <v>3</v>
+      </c>
       <c r="B13" s="23" t="s">
         <v>119</v>
       </c>
@@ -2785,10 +2791,10 @@
         <v>193</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" s="23" t="s">
         <v>120</v>
       </c>
@@ -2802,7 +2808,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="12">
         <v>1</v>
       </c>
@@ -2819,7 +2825,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="12">
         <v>1</v>
       </c>
@@ -2836,7 +2842,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" s="23" t="s">
         <v>138</v>
       </c>
@@ -2850,7 +2856,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="12">
         <v>1</v>
       </c>
@@ -2867,7 +2873,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="12">
         <v>1</v>
       </c>
@@ -2884,7 +2890,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="12">
         <v>3</v>
       </c>
@@ -2901,7 +2907,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="12">
         <v>2</v>
       </c>
@@ -2918,7 +2924,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B22" s="27" t="s">
         <v>136</v>
       </c>
@@ -2932,7 +2938,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="12">
         <v>2</v>
       </c>
@@ -2949,7 +2955,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="12">
         <v>3</v>
       </c>
@@ -2966,7 +2972,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B25" s="27" t="s">
         <v>153</v>
       </c>
@@ -2980,7 +2986,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B26" s="25" t="s">
         <v>121</v>
       </c>
@@ -2994,7 +3000,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="12">
         <v>3</v>
       </c>
@@ -3011,7 +3017,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="12">
         <v>1</v>
       </c>
@@ -3028,7 +3034,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="12">
         <v>3</v>
       </c>
@@ -3045,7 +3051,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="12">
         <v>2</v>
       </c>
@@ -3062,7 +3068,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="12">
         <v>2</v>
       </c>
@@ -3079,7 +3085,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -3096,7 +3102,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B33" s="25" t="s">
         <v>155</v>
       </c>
@@ -3110,7 +3116,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B34" s="34" t="s">
         <v>124</v>
       </c>
@@ -3124,7 +3130,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B35" s="34" t="s">
         <v>125</v>
       </c>
@@ -3138,7 +3144,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -3155,7 +3161,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="12">
         <v>2</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="12">
         <v>2</v>
       </c>
@@ -3189,7 +3195,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="12">
         <v>1</v>
       </c>
@@ -3206,7 +3212,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="12">
         <v>1</v>
       </c>
@@ -3223,7 +3229,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B41" s="34" t="s">
         <v>208</v>
       </c>
@@ -3237,7 +3243,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="12">
         <v>2</v>
       </c>
@@ -3254,7 +3260,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B43" s="38" t="s">
         <v>137</v>
       </c>
@@ -3268,7 +3274,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B44" s="38" t="s">
         <v>139</v>
       </c>
@@ -3282,7 +3288,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B45" s="38" t="s">
         <v>150</v>
       </c>
@@ -3296,7 +3302,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B46" s="38" t="s">
         <v>154</v>
       </c>
@@ -3310,7 +3316,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="12">
         <v>1</v>
       </c>
@@ -3327,7 +3333,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="12">
         <v>2</v>
       </c>
@@ -3344,7 +3350,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="12">
         <v>1</v>
       </c>
@@ -3361,7 +3367,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B50" s="39"/>
     </row>
   </sheetData>
@@ -3384,47 +3390,47 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="5"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3447,7 +3453,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3463,7 +3469,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3488,7 +3494,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>164</v>
       </c>
@@ -3513,7 +3519,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>165</v>
       </c>
@@ -3538,7 +3544,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>166</v>
       </c>
@@ -3578,17 +3584,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3608,7 +3614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="16">
         <v>42633</v>
       </c>
@@ -3622,7 +3628,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="16">
         <v>42647</v>
       </c>
@@ -3643,7 +3649,7 @@
         <v>30.054446460980031</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="16">
         <v>42654</v>
       </c>
@@ -3666,7 +3672,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="16">
         <v>42668</v>
       </c>
@@ -3681,7 +3687,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="16">
         <v>42683</v>
       </c>
@@ -3691,7 +3697,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="16">
         <v>42708</v>
       </c>
@@ -3701,7 +3707,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="16">
         <v>42728</v>
       </c>
@@ -3727,21 +3733,21 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="11" style="12"/>
-    <col min="5" max="5" width="6.875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="12" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="6.625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -3770,7 +3776,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>142</v>
       </c>
@@ -3799,7 +3805,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>143</v>
       </c>
@@ -3828,7 +3834,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>144</v>
       </c>
@@ -3857,7 +3863,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>130</v>
       </c>
@@ -3886,7 +3892,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>134</v>
       </c>
@@ -3915,7 +3921,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>123</v>
       </c>
@@ -3944,7 +3950,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>152</v>
       </c>
@@ -3973,7 +3979,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>117</v>
       </c>
@@ -4002,7 +4008,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>118</v>
       </c>
@@ -4031,7 +4037,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>206</v>
       </c>
@@ -4060,7 +4066,7 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>207</v>
       </c>
@@ -4089,7 +4095,7 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>126</v>
       </c>
@@ -4118,7 +4124,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>220</v>
       </c>
@@ -4147,7 +4153,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
         <v>222</v>
       </c>
@@ -4176,35 +4182,35 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="13" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="13" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="13" t="s">
         <v>251</v>
       </c>
@@ -4221,15 +4227,15 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -4258,7 +4264,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>148</v>
       </c>
@@ -4287,7 +4293,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>149</v>
       </c>
@@ -4316,7 +4322,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>145</v>
       </c>
@@ -4345,7 +4351,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>135</v>
       </c>
@@ -4374,7 +4380,7 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>140</v>
       </c>
@@ -4403,7 +4409,7 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>129</v>
       </c>
@@ -4432,7 +4438,7 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>114</v>
       </c>
@@ -4443,7 +4449,7 @@
         <v>193</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E8" s="12">
         <v>60</v>
@@ -4451,11 +4457,17 @@
       <c r="F8" s="12">
         <v>100</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8" s="12">
+        <v>23</v>
+      </c>
+      <c r="H8" s="12">
+        <v>30</v>
+      </c>
+      <c r="I8" s="50">
+        <v>42668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>115</v>
       </c>
@@ -4466,7 +4478,7 @@
         <v>193</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E9" s="12">
         <v>60</v>
@@ -4474,11 +4486,17 @@
       <c r="F9" s="12">
         <v>100</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G9" s="12">
+        <v>17</v>
+      </c>
+      <c r="H9" s="12">
+        <v>30</v>
+      </c>
+      <c r="I9" s="50">
+        <v>42668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>133</v>
       </c>
@@ -4501,7 +4519,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>221</v>
       </c>
@@ -4524,7 +4542,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>131</v>
       </c>
@@ -4547,7 +4565,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>132</v>
       </c>
@@ -4570,63 +4588,63 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="53"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="51"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="D21" s="54"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="54" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="52" t="s">
         <v>256</v>
       </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54" t="s">
+      <c r="D22" s="52"/>
+      <c r="E22" s="52" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="54" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="52" t="s">
         <v>257</v>
       </c>
-      <c r="E23" s="54" t="s">
+      <c r="E23" s="52" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="54" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="52" t="s">
         <v>258</v>
       </c>
-      <c r="E24" s="54" t="s">
+      <c r="E24" s="52" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="54" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="52" t="s">
         <v>261</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="52" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="54" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="52" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="54" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="52" t="s">
         <v>267</v>
       </c>
     </row>
@@ -4639,18 +4657,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4679,7 +4697,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>128</v>
       </c>
@@ -4702,7 +4720,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>147</v>
       </c>
@@ -4725,7 +4743,7 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>122</v>
       </c>
@@ -4748,7 +4766,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>127</v>
       </c>
@@ -4771,7 +4789,7 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
         <v>146</v>
       </c>
@@ -4794,7 +4812,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
         <v>151</v>
       </c>
@@ -4817,27 +4835,56 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" s="12">
+        <v>30</v>
+      </c>
+      <c r="F8" s="12">
+        <v>60</v>
+      </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="12">
+        <v>30</v>
+      </c>
+      <c r="F9" s="12">
+        <v>60</v>
+      </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4853,12 +4900,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4901,13 +4948,13 @@
       <selection activeCell="A36" sqref="A36:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>113</v>
       </c>
@@ -4918,7 +4965,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="23" t="s">
         <v>114</v>
       </c>
@@ -4929,7 +4976,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
         <v>115</v>
       </c>
@@ -4940,7 +4987,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
         <v>116</v>
       </c>
@@ -4951,7 +4998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" s="27" t="s">
         <v>117</v>
       </c>
@@ -4962,7 +5009,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" s="27" t="s">
         <v>118</v>
       </c>
@@ -4973,7 +5020,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="23" t="s">
         <v>119</v>
       </c>
@@ -4984,7 +5031,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="31" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="31" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" s="23" t="s">
         <v>120</v>
       </c>
@@ -4995,7 +5042,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" s="25" t="s">
         <v>121</v>
       </c>
@@ -5006,7 +5053,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="25" t="s">
         <v>122</v>
       </c>
@@ -5017,7 +5064,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
         <v>123</v>
       </c>
@@ -5028,7 +5075,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="34" t="s">
         <v>124</v>
       </c>
@@ -5039,7 +5086,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" s="34" t="s">
         <v>125</v>
       </c>
@@ -5050,7 +5097,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="36" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" s="34" t="s">
         <v>126</v>
       </c>
@@ -5061,7 +5108,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
         <v>127</v>
       </c>
@@ -5072,7 +5119,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="27" t="s">
         <v>128</v>
       </c>
@@ -5083,7 +5130,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="27" t="s">
         <v>129</v>
       </c>
@@ -5094,7 +5141,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" s="23" t="s">
         <v>130</v>
       </c>
@@ -5105,7 +5152,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="34" t="s">
         <v>131</v>
       </c>
@@ -5116,7 +5163,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="34" t="s">
         <v>132</v>
       </c>
@@ -5127,7 +5174,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="38" t="s">
         <v>133</v>
       </c>
@@ -5138,7 +5185,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="23" t="s">
         <v>134</v>
       </c>
@@ -5149,7 +5196,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" s="25" t="s">
         <v>135</v>
       </c>
@@ -5160,7 +5207,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" s="27" t="s">
         <v>136</v>
       </c>
@@ -5171,7 +5218,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="37" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="37" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="38" t="s">
         <v>137</v>
       </c>
@@ -5182,7 +5229,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="23" t="s">
         <v>138</v>
       </c>
@@ -5193,7 +5240,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="37" customFormat="1" ht="110.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="37" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A27" s="38" t="s">
         <v>139</v>
       </c>
@@ -5204,7 +5251,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="27" t="s">
         <v>140</v>
       </c>
@@ -5215,7 +5262,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" s="21" t="s">
         <v>141</v>
       </c>
@@ -5226,7 +5273,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="21" t="s">
         <v>142</v>
       </c>
@@ -5237,7 +5284,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="21" t="s">
         <v>143</v>
       </c>
@@ -5248,7 +5295,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="21" t="s">
         <v>144</v>
       </c>
@@ -5259,7 +5306,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="25" t="s">
         <v>145</v>
       </c>
@@ -5270,7 +5317,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" s="21" t="s">
         <v>146</v>
       </c>
@@ -5281,7 +5328,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" s="27" t="s">
         <v>147</v>
       </c>
@@ -5292,7 +5339,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" s="21" t="s">
         <v>148</v>
       </c>
@@ -5303,7 +5350,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" s="21" t="s">
         <v>149</v>
       </c>
@@ -5314,7 +5361,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" s="38" t="s">
         <v>150</v>
       </c>
@@ -5325,7 +5372,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" s="21" t="s">
         <v>151</v>
       </c>
@@ -5336,7 +5383,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" s="25" t="s">
         <v>152</v>
       </c>
@@ -5347,7 +5394,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" s="27" t="s">
         <v>153</v>
       </c>
@@ -5358,7 +5405,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" s="38" t="s">
         <v>154</v>
       </c>
@@ -5369,7 +5416,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" s="25" t="s">
         <v>155</v>
       </c>
@@ -5380,7 +5427,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A44" s="34" t="s">
         <v>206</v>
       </c>
@@ -5391,7 +5438,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A45" s="34" t="s">
         <v>207</v>
       </c>
@@ -5402,7 +5449,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A46" s="34" t="s">
         <v>208</v>
       </c>
@@ -5413,7 +5460,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="38" t="s">
         <v>220</v>
       </c>
@@ -5424,7 +5471,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" s="38" t="s">
         <v>221</v>
       </c>
@@ -5435,7 +5482,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="38" t="s">
         <v>222</v>
       </c>

</xml_diff>

<commit_message>
Updated Burndown Chart for Sprint 2 - Pradeep
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuragaman/Desktop/StudentID#10446036/CS_555_Project-master 2/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53958FE-419E-CD4E-8487-F03AB6B0C78D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -27,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$E$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Stories!$A$1:$C$43</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -761,9 +755,6 @@
     <t>List people with single parent</t>
   </si>
   <si>
-    <t>List all people in a GEDCOM file who have either their father or their mother died in last 30 days</t>
-  </si>
-  <si>
     <t>List living Single (Paired Programming)</t>
   </si>
   <si>
@@ -879,12 +870,15 @@
   </si>
   <si>
     <t>6. Update testdata for each usecase</t>
+  </si>
+  <si>
+    <t>List all people in a GEDCOM file who have either their father or their mother</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1126,7 +1120,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1206,6 +1200,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1300,7 +1295,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1326,7 +1321,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1371,7 +1366,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B4BC-4DF7-BB23-B148409AC56E}"/>
             </c:ext>
@@ -1387,28 +1382,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="212443136"/>
-        <c:axId val="212444672"/>
+        <c:axId val="207335808"/>
+        <c:axId val="207337344"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="212443136"/>
+        <c:axId val="207335808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212444672"/>
+        <c:crossAx val="207337344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="212444672"/>
+        <c:axId val="207337344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1419,7 +1414,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212443136"/>
+        <c:crossAx val="207335808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1437,7 +1432,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1511,7 +1506,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C9EC-4DFB-9A9C-08D916B18EAB}"/>
             </c:ext>
@@ -1527,11 +1522,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="213431424"/>
-        <c:axId val="213432960"/>
+        <c:axId val="208311808"/>
+        <c:axId val="208313344"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="213431424"/>
+        <c:axId val="208311808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,14 +1536,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213432960"/>
+        <c:crossAx val="208313344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="213432960"/>
+        <c:axId val="208313344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213431424"/>
+        <c:crossAx val="208311808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1596,7 +1591,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1634,7 +1629,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1709,7 +1704,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1774,7 +1769,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1843,7 +1838,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1913,7 +1908,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1982,7 +1977,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2052,7 +2047,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2392,23 +2387,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="12" customWidth="1"/>
-    <col min="4" max="5" width="20.5" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="12" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" style="12" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
@@ -2425,7 +2420,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>192</v>
       </c>
@@ -2442,7 +2437,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>193</v>
       </c>
@@ -2459,7 +2454,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>194</v>
       </c>
@@ -2476,7 +2471,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>195</v>
       </c>
@@ -2493,7 +2488,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>201</v>
       </c>
@@ -2510,7 +2505,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>215</v>
       </c>
@@ -2527,19 +2522,19 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="F9" s="53"/>
-      <c r="G9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="55"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
+  <sortState ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <mergeCells count="1">
@@ -2547,12 +2542,12 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId7"/>
@@ -2560,23 +2555,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C13"/>
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.6328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
@@ -2593,7 +2588,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2610,7 +2605,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -2627,7 +2622,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>141</v>
       </c>
@@ -2641,7 +2636,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -2658,7 +2653,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -2675,7 +2670,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -2692,7 +2687,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>2</v>
       </c>
@@ -2709,7 +2704,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>3</v>
       </c>
@@ -2726,7 +2721,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>2</v>
       </c>
@@ -2743,7 +2738,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>2</v>
       </c>
@@ -2760,7 +2755,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>3</v>
       </c>
@@ -2777,7 +2772,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>3</v>
       </c>
@@ -2794,7 +2789,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>120</v>
       </c>
@@ -2808,7 +2803,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>1</v>
       </c>
@@ -2825,7 +2820,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>1</v>
       </c>
@@ -2842,7 +2837,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>138</v>
       </c>
@@ -2856,7 +2851,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>1</v>
       </c>
@@ -2873,7 +2868,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>1</v>
       </c>
@@ -2890,7 +2885,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>3</v>
       </c>
@@ -2907,7 +2902,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>2</v>
       </c>
@@ -2924,7 +2919,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>136</v>
       </c>
@@ -2938,7 +2933,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>2</v>
       </c>
@@ -2955,7 +2950,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>3</v>
       </c>
@@ -2972,7 +2967,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
         <v>153</v>
       </c>
@@ -2986,7 +2981,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
         <v>121</v>
       </c>
@@ -3000,7 +2995,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>3</v>
       </c>
@@ -3017,7 +3012,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>1</v>
       </c>
@@ -3034,7 +3029,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>3</v>
       </c>
@@ -3051,7 +3046,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>2</v>
       </c>
@@ -3068,7 +3063,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>2</v>
       </c>
@@ -3085,7 +3080,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -3102,7 +3097,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
         <v>155</v>
       </c>
@@ -3116,7 +3111,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" s="34" t="s">
         <v>124</v>
       </c>
@@ -3130,7 +3125,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="34" t="s">
         <v>125</v>
       </c>
@@ -3144,7 +3139,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -3152,7 +3147,7 @@
         <v>126</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>201</v>
@@ -3161,7 +3156,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>2</v>
       </c>
@@ -3178,7 +3173,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>2</v>
       </c>
@@ -3195,7 +3190,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>1</v>
       </c>
@@ -3212,7 +3207,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>1</v>
       </c>
@@ -3220,7 +3215,7 @@
         <v>207</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>201</v>
@@ -3229,7 +3224,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="34" t="s">
         <v>208</v>
       </c>
@@ -3243,7 +3238,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>2</v>
       </c>
@@ -3260,7 +3255,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="38" t="s">
         <v>137</v>
       </c>
@@ -3274,7 +3269,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="38" t="s">
         <v>139</v>
       </c>
@@ -3288,7 +3283,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="38" t="s">
         <v>150</v>
       </c>
@@ -3302,7 +3297,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="38" t="s">
         <v>154</v>
       </c>
@@ -3316,7 +3311,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>1</v>
       </c>
@@ -3333,7 +3328,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>2</v>
       </c>
@@ -3347,10 +3342,10 @@
         <v>215</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>1</v>
       </c>
@@ -3367,12 +3362,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" s="39"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E25" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">
+  <autoFilter ref="A1:E25">
+    <sortState ref="A2:E25">
       <sortCondition ref="A1:A25"/>
     </sortState>
   </autoFilter>
@@ -3383,54 +3378,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="5"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3453,7 +3448,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3469,7 +3464,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3494,7 +3489,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>164</v>
       </c>
@@ -3519,7 +3514,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>165</v>
       </c>
@@ -3544,7 +3539,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>166</v>
       </c>
@@ -3577,24 +3572,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3614,7 +3609,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>42633</v>
       </c>
@@ -3628,7 +3623,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>42647</v>
       </c>
@@ -3649,7 +3644,7 @@
         <v>30.054446460980031</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>42654</v>
       </c>
@@ -3669,10 +3664,10 @@
         <v>30.1</v>
       </c>
       <c r="G4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>42668</v>
       </c>
@@ -3687,7 +3682,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>42683</v>
       </c>
@@ -3697,7 +3692,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>42708</v>
       </c>
@@ -3707,7 +3702,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>42728</v>
       </c>
@@ -3726,28 +3721,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="27.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" style="12" customWidth="1"/>
     <col min="4" max="4" width="11" style="12"/>
-    <col min="5" max="5" width="6.83203125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="6.6328125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.6328125" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -3776,7 +3771,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>142</v>
       </c>
@@ -3805,7 +3800,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>143</v>
       </c>
@@ -3834,15 +3829,15 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>144</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>229</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>230</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>200</v>
@@ -3863,12 +3858,12 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>130</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>193</v>
@@ -3892,15 +3887,15 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>134</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>200</v>
@@ -3921,7 +3916,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>123</v>
       </c>
@@ -3950,7 +3945,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>152</v>
       </c>
@@ -3979,7 +3974,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>117</v>
       </c>
@@ -4008,7 +4003,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>118</v>
       </c>
@@ -4037,12 +4032,12 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>206</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>201</v>
@@ -4066,12 +4061,12 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>207</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>201</v>
@@ -4095,12 +4090,12 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>126</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>201</v>
@@ -4124,12 +4119,12 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>220</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>215</v>
@@ -4153,12 +4148,12 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>222</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>215</v>
@@ -4182,37 +4177,37 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B20" s="13" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -4223,19 +4218,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -4264,7 +4259,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>148</v>
       </c>
@@ -4293,7 +4288,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>149</v>
       </c>
@@ -4322,7 +4317,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>145</v>
       </c>
@@ -4351,7 +4346,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>135</v>
       </c>
@@ -4380,12 +4375,12 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>140</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>195</v>
@@ -4409,12 +4404,12 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>129</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>195</v>
@@ -4438,12 +4433,12 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>114</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>193</v>
@@ -4467,12 +4462,12 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>115</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>193</v>
@@ -4496,12 +4491,12 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>133</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>215</v>
@@ -4510,7 +4505,7 @@
         <v>199</v>
       </c>
       <c r="E10" s="12">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F10" s="12">
         <v>100</v>
@@ -4519,12 +4514,12 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>221</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>215</v>
@@ -4538,16 +4533,22 @@
       <c r="F11" s="12">
         <v>100</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G11" s="12">
+        <v>16</v>
+      </c>
+      <c r="H11" s="12">
+        <v>30</v>
+      </c>
+      <c r="I11" s="53">
+        <v>42668</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>131</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>201</v>
@@ -4565,12 +4566,12 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>132</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>201</v>
@@ -4588,64 +4589,64 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="51"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D21" s="52"/>
       <c r="E21" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D22" s="52"/>
       <c r="E22" s="52" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="E23" s="52" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
+        <v>257</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="52" t="s">
+        <v>260</v>
+      </c>
+      <c r="E25" s="52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="52" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="52" t="s">
-        <v>257</v>
-      </c>
-      <c r="E23" s="52" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="52" t="s">
-        <v>258</v>
-      </c>
-      <c r="E24" s="52" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="52" t="s">
-        <v>261</v>
-      </c>
-      <c r="E25" s="52" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="52" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="52" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="52" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -4656,19 +4657,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4697,12 +4698,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>195</v>
@@ -4720,12 +4721,12 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>147</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>195</v>
@@ -4743,7 +4744,7 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>122</v>
       </c>
@@ -4766,7 +4767,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>127</v>
       </c>
@@ -4789,7 +4790,7 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>146</v>
       </c>
@@ -4812,7 +4813,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>151</v>
       </c>
@@ -4835,7 +4836,7 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>116</v>
       </c>
@@ -4858,7 +4859,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>119</v>
       </c>
@@ -4881,7 +4882,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="33"/>
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
@@ -4893,19 +4894,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4941,20 +4942,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:C37"/>
+    <sheetView topLeftCell="A36" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>113</v>
       </c>
@@ -4965,7 +4966,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>114</v>
       </c>
@@ -4976,7 +4977,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>115</v>
       </c>
@@ -4987,7 +4988,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>116</v>
       </c>
@@ -4998,7 +4999,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>117</v>
       </c>
@@ -5009,7 +5010,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>118</v>
       </c>
@@ -5020,7 +5021,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>119</v>
       </c>
@@ -5031,7 +5032,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="31" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" s="31" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>120</v>
       </c>
@@ -5042,7 +5043,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>121</v>
       </c>
@@ -5053,7 +5054,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>122</v>
       </c>
@@ -5064,7 +5065,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>123</v>
       </c>
@@ -5075,7 +5076,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>124</v>
       </c>
@@ -5086,7 +5087,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>125</v>
       </c>
@@ -5097,7 +5098,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="36" customFormat="1" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" s="36" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>126</v>
       </c>
@@ -5108,7 +5109,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>127</v>
       </c>
@@ -5119,7 +5120,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>128</v>
       </c>
@@ -5130,7 +5131,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>129</v>
       </c>
@@ -5141,7 +5142,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>130</v>
       </c>
@@ -5152,7 +5153,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>131</v>
       </c>
@@ -5163,7 +5164,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>132</v>
       </c>
@@ -5174,7 +5175,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>133</v>
       </c>
@@ -5185,7 +5186,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>134</v>
       </c>
@@ -5196,7 +5197,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>135</v>
       </c>
@@ -5207,7 +5208,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>136</v>
       </c>
@@ -5218,7 +5219,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="37" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" s="37" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
         <v>137</v>
       </c>
@@ -5229,7 +5230,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>138</v>
       </c>
@@ -5240,7 +5241,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="37" customFormat="1" ht="119" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" s="37" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
         <v>139</v>
       </c>
@@ -5251,7 +5252,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>140</v>
       </c>
@@ -5262,7 +5263,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>141</v>
       </c>
@@ -5273,7 +5274,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>142</v>
       </c>
@@ -5284,7 +5285,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>143</v>
       </c>
@@ -5295,7 +5296,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>144</v>
       </c>
@@ -5306,7 +5307,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>145</v>
       </c>
@@ -5317,7 +5318,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>146</v>
       </c>
@@ -5328,7 +5329,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>147</v>
       </c>
@@ -5339,7 +5340,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>148</v>
       </c>
@@ -5350,7 +5351,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>149</v>
       </c>
@@ -5361,7 +5362,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" s="37" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
         <v>150</v>
       </c>
@@ -5372,7 +5373,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>151</v>
       </c>
@@ -5383,7 +5384,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>152</v>
       </c>
@@ -5394,7 +5395,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>153</v>
       </c>
@@ -5405,7 +5406,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A42" s="38" t="s">
         <v>154</v>
       </c>
@@ -5416,7 +5417,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>155</v>
       </c>
@@ -5427,7 +5428,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A44" s="34" t="s">
         <v>206</v>
       </c>
@@ -5438,7 +5439,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A45" s="34" t="s">
         <v>207</v>
       </c>
@@ -5449,7 +5450,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A46" s="34" t="s">
         <v>208</v>
       </c>
@@ -5460,7 +5461,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="38" t="s">
         <v>220</v>
       </c>
@@ -5471,7 +5472,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" s="37" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A48" s="38" t="s">
         <v>221</v>
       </c>
@@ -5479,10 +5480,10 @@
         <v>227</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="38" t="s">
         <v>222</v>
       </c>
@@ -5494,7 +5495,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C43" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
+  <autoFilter ref="A1:C43"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>

<commit_message>
US20 Completed and Updated Burndown chart
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="268">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1120,7 +1120,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1200,7 +1200,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1382,11 +1381,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="207335808"/>
-        <c:axId val="207337344"/>
+        <c:axId val="205304192"/>
+        <c:axId val="205305728"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="207335808"/>
+        <c:axId val="205304192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1396,14 +1395,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="207337344"/>
+        <c:crossAx val="205305728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="207337344"/>
+        <c:axId val="205305728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1414,7 +1413,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="207335808"/>
+        <c:crossAx val="205304192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1522,11 +1521,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="208311808"/>
-        <c:axId val="208313344"/>
+        <c:axId val="206284288"/>
+        <c:axId val="206285824"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="208311808"/>
+        <c:axId val="206284288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1536,14 +1535,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208313344"/>
+        <c:crossAx val="206285824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="208313344"/>
+        <c:axId val="206285824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,7 +1553,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208311808"/>
+        <c:crossAx val="206284288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1591,7 +1590,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1629,7 +1628,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1704,7 +1703,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1769,7 +1768,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1838,7 +1837,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1908,7 +1907,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1977,7 +1976,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2047,7 +2046,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2527,11 +2526,11 @@
       <c r="D9" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="54"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -2559,7 +2558,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3252,10 +3251,13 @@
         <v>215</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="12">
+        <v>3</v>
+      </c>
       <c r="B43" s="38" t="s">
         <v>137</v>
       </c>
@@ -3266,10 +3268,13 @@
         <v>215</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="12">
+        <v>3</v>
+      </c>
       <c r="B44" s="38" t="s">
         <v>139</v>
       </c>
@@ -3280,7 +3285,7 @@
         <v>215</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -4221,8 +4226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4502,7 +4507,7 @@
         <v>215</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E10" s="12">
         <v>60</v>
@@ -4510,9 +4515,15 @@
       <c r="F10" s="12">
         <v>100</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="G10" s="12">
+        <v>62</v>
+      </c>
+      <c r="H10" s="12">
+        <v>45</v>
+      </c>
+      <c r="I10" s="50">
+        <v>42671</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
@@ -4525,7 +4536,7 @@
         <v>215</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E11" s="12">
         <v>40</v>
@@ -4539,7 +4550,7 @@
       <c r="H11" s="12">
         <v>30</v>
       </c>
-      <c r="I11" s="53">
+      <c r="I11" s="50">
         <v>42668</v>
       </c>
     </row>
@@ -4658,10 +4669,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4883,9 +4894,44 @@
       <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
+      <c r="A10" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" s="12">
+        <v>50</v>
+      </c>
+      <c r="F10" s="12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E11" s="12">
+        <v>60</v>
+      </c>
+      <c r="F11" s="12">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4945,8 +4991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated status of sprint 3 user story 33 and 38 and its actual time and LOC. And points for keep doing and Avoid in Sprint 3 sheet
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neil Naidu\Desktop\CS Sem 1\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88187F4-9154-46FF-892E-161179C1FABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C78546E-D8E5-4376-8CA4-EE99E7D9291B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="274">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -886,6 +885,18 @@
   </si>
   <si>
     <t>No Bigamy</t>
+  </si>
+  <si>
+    <t>7. Identify bugs/defects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Prioritize and fix bugd/defetcs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. Lend helping hands to other developers, if required </t>
+  </si>
+  <si>
+    <t>5. Keep standup calls short and specific to the point</t>
   </si>
 </sst>
 </file>
@@ -2580,8 +2591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2645,6 +2656,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>4</v>
+      </c>
       <c r="B4" s="21" t="s">
         <v>141</v>
       </c>
@@ -2655,7 +2669,7 @@
         <v>192</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2689,7 +2703,7 @@
         <v>192</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2740,7 +2754,7 @@
         <v>192</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -3569,7 +3583,7 @@
         <v>160</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" ref="G17:G19" si="1">(E18-E17)/F18*60</f>
+        <f t="shared" ref="G18:G19" si="1">(E18-E17)/F18*60</f>
         <v>97.5</v>
       </c>
     </row>
@@ -4261,8 +4275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H33" sqref="A20:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4716,10 +4730,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4859,7 +4873,7 @@
         <v>192</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E6" s="12">
         <v>25</v>
@@ -4867,9 +4881,15 @@
       <c r="F6" s="12">
         <v>60</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="G6" s="12">
+        <v>41</v>
+      </c>
+      <c r="H6" s="12">
+        <v>100</v>
+      </c>
+      <c r="I6" s="50">
+        <v>42682</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
@@ -4882,7 +4902,7 @@
         <v>192</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E7" s="12">
         <v>25</v>
@@ -4890,9 +4910,15 @@
       <c r="F7" s="12">
         <v>60</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="12">
+        <v>24</v>
+      </c>
+      <c r="H7" s="12">
+        <v>60</v>
+      </c>
+      <c r="I7" s="50">
+        <v>42682</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
@@ -5018,6 +5044,81 @@
       </c>
       <c r="F13" s="12">
         <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="52"/>
+      <c r="E20" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="52" t="s">
+        <v>255</v>
+      </c>
+      <c r="E22" s="52" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="E23" s="52" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
+        <v>259</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="52" t="s">
+        <v>261</v>
+      </c>
+      <c r="E25" s="52" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="52" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="52" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="52" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -5028,15 +5129,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="11" style="12"/>
+    <col min="1" max="1" width="11" style="12"/>
+    <col min="2" max="2" width="15.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -5066,6 +5169,26 @@
       </c>
       <c r="I1" s="19" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="12">
+        <v>40</v>
+      </c>
+      <c r="F2" s="12">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -5078,8 +5201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated the details with relevant information
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuragaman/Desktop/CS_555_Project-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C78546E-D8E5-4376-8CA4-EE99E7D9291B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4C78CA-649E-F84C-9705-32CB8653E4D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="274">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1344,7 +1344,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1415,7 +1415,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2427,16 +2427,16 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="12" customWidth="1"/>
     <col min="4" max="5" width="20.5" style="12" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="21" t="s">
         <v>192</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
         <v>193</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="25" t="s">
         <v>194</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="27" t="s">
         <v>195</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="34" t="s">
         <v>201</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="38" t="s">
         <v>215</v>
       </c>
@@ -2555,8 +2555,8 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="D9" s="35" t="s">
         <v>34</v>
       </c>
@@ -2591,20 +2591,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="6.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>4</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>2</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>3</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>2</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>2</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>3</v>
       </c>
@@ -2805,10 +2805,10 @@
         <v>193</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
         <v>3</v>
       </c>
@@ -2822,10 +2822,13 @@
         <v>193</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="12">
+        <v>4</v>
+      </c>
       <c r="B14" s="23" t="s">
         <v>120</v>
       </c>
@@ -2836,10 +2839,10 @@
         <v>193</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="12">
         <v>1</v>
       </c>
@@ -2856,7 +2859,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="12">
         <v>1</v>
       </c>
@@ -2873,7 +2876,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="12">
+        <v>4</v>
+      </c>
       <c r="B17" s="23" t="s">
         <v>138</v>
       </c>
@@ -2884,10 +2890,10 @@
         <v>193</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="12">
         <v>1</v>
       </c>
@@ -2904,7 +2910,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="12">
         <v>1</v>
       </c>
@@ -2921,7 +2927,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="12">
         <v>3</v>
       </c>
@@ -2938,7 +2944,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="12">
         <v>2</v>
       </c>
@@ -2955,7 +2961,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B22" s="27" t="s">
         <v>136</v>
       </c>
@@ -2969,7 +2975,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="12">
         <v>2</v>
       </c>
@@ -2986,7 +2992,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="12">
         <v>3</v>
       </c>
@@ -3003,7 +3009,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B25" s="27" t="s">
         <v>153</v>
       </c>
@@ -3017,7 +3023,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B26" s="25" t="s">
         <v>121</v>
       </c>
@@ -3031,7 +3037,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="12">
         <v>3</v>
       </c>
@@ -3048,7 +3054,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="12">
         <v>1</v>
       </c>
@@ -3065,7 +3071,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="12">
         <v>3</v>
       </c>
@@ -3082,7 +3088,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="12">
         <v>2</v>
       </c>
@@ -3099,7 +3105,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="12">
         <v>2</v>
       </c>
@@ -3116,7 +3122,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -3133,7 +3139,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B33" s="25" t="s">
         <v>155</v>
       </c>
@@ -3147,7 +3153,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="12">
         <v>3</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="12">
         <v>3</v>
       </c>
@@ -3181,7 +3187,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -3198,7 +3204,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="12">
         <v>2</v>
       </c>
@@ -3215,7 +3221,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="12">
         <v>2</v>
       </c>
@@ -3232,7 +3238,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="12">
         <v>1</v>
       </c>
@@ -3249,7 +3255,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="12">
         <v>1</v>
       </c>
@@ -3266,7 +3272,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B41" s="34" t="s">
         <v>208</v>
       </c>
@@ -3280,7 +3286,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="12">
         <v>2</v>
       </c>
@@ -3297,7 +3303,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="12">
         <v>3</v>
       </c>
@@ -3314,7 +3320,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="12">
         <v>3</v>
       </c>
@@ -3331,7 +3337,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B45" s="38" t="s">
         <v>150</v>
       </c>
@@ -3345,7 +3351,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B46" s="38" t="s">
         <v>154</v>
       </c>
@@ -3359,7 +3365,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="12">
         <v>1</v>
       </c>
@@ -3376,7 +3382,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="12">
         <v>2</v>
       </c>
@@ -3393,7 +3399,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="12">
         <v>1</v>
       </c>
@@ -3410,7 +3416,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B50" s="39"/>
     </row>
   </sheetData>
@@ -3433,47 +3439,47 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="5"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3496,7 +3502,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3512,7 +3518,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3537,7 +3543,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>164</v>
       </c>
@@ -3562,7 +3568,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>165</v>
       </c>
@@ -3587,7 +3593,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>166</v>
       </c>
@@ -3627,17 +3633,17 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3657,7 +3663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="16">
         <v>42633</v>
       </c>
@@ -3671,7 +3677,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="16">
         <v>42647</v>
       </c>
@@ -3692,7 +3698,7 @@
         <v>30.054446460980031</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="16">
         <v>42654</v>
       </c>
@@ -3715,7 +3721,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="16">
         <v>42668</v>
       </c>
@@ -3736,7 +3742,7 @@
         <v>69.697999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="16">
         <v>42683</v>
       </c>
@@ -3746,7 +3752,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="16">
         <v>42708</v>
       </c>
@@ -3756,7 +3762,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="16">
         <v>42728</v>
       </c>
@@ -3782,21 +3788,21 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="11" style="12"/>
-    <col min="5" max="5" width="6.875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="12" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="6.625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -3825,7 +3831,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>142</v>
       </c>
@@ -3854,7 +3860,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>143</v>
       </c>
@@ -3883,7 +3889,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>144</v>
       </c>
@@ -3912,7 +3918,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>130</v>
       </c>
@@ -3941,7 +3947,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>134</v>
       </c>
@@ -3970,7 +3976,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>123</v>
       </c>
@@ -3999,7 +4005,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>152</v>
       </c>
@@ -4028,7 +4034,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>117</v>
       </c>
@@ -4057,7 +4063,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>118</v>
       </c>
@@ -4086,7 +4092,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>206</v>
       </c>
@@ -4115,7 +4121,7 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>207</v>
       </c>
@@ -4144,7 +4150,7 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>126</v>
       </c>
@@ -4173,7 +4179,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>220</v>
       </c>
@@ -4202,7 +4208,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
         <v>222</v>
       </c>
@@ -4231,35 +4237,35 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="13" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="13" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="13" t="s">
         <v>249</v>
       </c>
@@ -4276,15 +4282,15 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H33" sqref="A20:H33"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -4313,7 +4319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>148</v>
       </c>
@@ -4342,7 +4348,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>149</v>
       </c>
@@ -4371,7 +4377,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>145</v>
       </c>
@@ -4400,7 +4406,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>135</v>
       </c>
@@ -4429,7 +4435,7 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>140</v>
       </c>
@@ -4458,7 +4464,7 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>129</v>
       </c>
@@ -4487,7 +4493,7 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>114</v>
       </c>
@@ -4516,7 +4522,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>115</v>
       </c>
@@ -4545,7 +4551,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>133</v>
       </c>
@@ -4574,7 +4580,7 @@
         <v>42671</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>221</v>
       </c>
@@ -4603,7 +4609,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>131</v>
       </c>
@@ -4632,7 +4638,7 @@
         <v>42672</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>132</v>
       </c>
@@ -4661,15 +4667,15 @@
         <v>42673</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="51"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>258</v>
       </c>
@@ -4678,7 +4684,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="52" t="s">
         <v>254</v>
       </c>
@@ -4687,7 +4693,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="52" t="s">
         <v>255</v>
       </c>
@@ -4695,7 +4701,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="52" t="s">
         <v>256</v>
       </c>
@@ -4703,7 +4709,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="52" t="s">
         <v>259</v>
       </c>
@@ -4711,12 +4717,12 @@
         <v>264</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="52" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="52" t="s">
         <v>265</v>
       </c>
@@ -4732,16 +4738,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4770,7 +4776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>128</v>
       </c>
@@ -4793,7 +4799,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>147</v>
       </c>
@@ -4816,7 +4822,7 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>122</v>
       </c>
@@ -4839,7 +4845,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>127</v>
       </c>
@@ -4862,7 +4868,7 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
         <v>146</v>
       </c>
@@ -4891,7 +4897,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
         <v>151</v>
       </c>
@@ -4920,7 +4926,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
         <v>116</v>
       </c>
@@ -4931,7 +4937,7 @@
         <v>193</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E8" s="12">
         <v>30</v>
@@ -4939,11 +4945,17 @@
       <c r="F8" s="12">
         <v>60</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8" s="12">
+        <v>35</v>
+      </c>
+      <c r="H8" s="12">
+        <v>60</v>
+      </c>
+      <c r="I8" s="50">
+        <v>42682</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
         <v>119</v>
       </c>
@@ -4954,7 +4966,7 @@
         <v>193</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E9" s="12">
         <v>30</v>
@@ -4962,11 +4974,17 @@
       <c r="F9" s="12">
         <v>60</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G9" s="12">
+        <v>32</v>
+      </c>
+      <c r="H9" s="12">
+        <v>70</v>
+      </c>
+      <c r="I9" s="50">
+        <v>42682</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
         <v>137</v>
       </c>
@@ -4986,7 +5004,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="33" t="s">
         <v>139</v>
       </c>
@@ -5006,7 +5024,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="33" t="s">
         <v>124</v>
       </c>
@@ -5026,7 +5044,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="33" t="s">
         <v>125</v>
       </c>
@@ -5046,12 +5064,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>258</v>
       </c>
@@ -5060,7 +5078,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="52" t="s">
         <v>254</v>
       </c>
@@ -5069,7 +5087,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="52" t="s">
         <v>255</v>
       </c>
@@ -5077,7 +5095,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="52" t="s">
         <v>256</v>
       </c>
@@ -5085,7 +5103,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="52" t="s">
         <v>259</v>
       </c>
@@ -5093,7 +5111,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="52" t="s">
         <v>261</v>
       </c>
@@ -5101,22 +5119,22 @@
         <v>273</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="52" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="52" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="52" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="52" t="s">
         <v>272</v>
       </c>
@@ -5129,20 +5147,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="12"/>
-    <col min="2" max="2" width="15.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -5171,7 +5189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>141</v>
       </c>
@@ -5189,6 +5207,46 @@
       </c>
       <c r="F2" s="12">
         <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" s="12">
+        <v>30</v>
+      </c>
+      <c r="F3" s="12">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4" s="12">
+        <v>30</v>
+      </c>
+      <c r="F4" s="12">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -5205,13 +5263,13 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>113</v>
       </c>
@@ -5222,7 +5280,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="23" t="s">
         <v>114</v>
       </c>
@@ -5233,7 +5291,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
         <v>115</v>
       </c>
@@ -5244,7 +5302,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
         <v>116</v>
       </c>
@@ -5255,7 +5313,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" s="27" t="s">
         <v>117</v>
       </c>
@@ -5266,7 +5324,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" s="27" t="s">
         <v>118</v>
       </c>
@@ -5277,7 +5335,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="23" t="s">
         <v>119</v>
       </c>
@@ -5288,7 +5346,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="31" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="31" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" s="23" t="s">
         <v>120</v>
       </c>
@@ -5299,7 +5357,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" s="25" t="s">
         <v>121</v>
       </c>
@@ -5310,7 +5368,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="25" t="s">
         <v>122</v>
       </c>
@@ -5321,7 +5379,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
         <v>123</v>
       </c>
@@ -5332,7 +5390,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="34" t="s">
         <v>124</v>
       </c>
@@ -5343,7 +5401,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" s="34" t="s">
         <v>125</v>
       </c>
@@ -5354,7 +5412,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="36" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" s="34" t="s">
         <v>126</v>
       </c>
@@ -5365,7 +5423,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
         <v>127</v>
       </c>
@@ -5376,7 +5434,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="27" t="s">
         <v>128</v>
       </c>
@@ -5387,7 +5445,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="27" t="s">
         <v>129</v>
       </c>
@@ -5398,7 +5456,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" s="23" t="s">
         <v>130</v>
       </c>
@@ -5409,7 +5467,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="34" t="s">
         <v>131</v>
       </c>
@@ -5420,7 +5478,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="34" t="s">
         <v>132</v>
       </c>
@@ -5431,7 +5489,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="38" t="s">
         <v>133</v>
       </c>
@@ -5442,7 +5500,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="23" t="s">
         <v>134</v>
       </c>
@@ -5453,7 +5511,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" s="25" t="s">
         <v>135</v>
       </c>
@@ -5464,7 +5522,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" s="27" t="s">
         <v>136</v>
       </c>
@@ -5475,7 +5533,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="37" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="37" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="38" t="s">
         <v>137</v>
       </c>
@@ -5486,7 +5544,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="23" t="s">
         <v>138</v>
       </c>
@@ -5497,7 +5555,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="37" customFormat="1" ht="110.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="37" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A27" s="38" t="s">
         <v>139</v>
       </c>
@@ -5508,7 +5566,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="27" t="s">
         <v>140</v>
       </c>
@@ -5519,7 +5577,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" s="21" t="s">
         <v>141</v>
       </c>
@@ -5530,7 +5588,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="21" t="s">
         <v>142</v>
       </c>
@@ -5541,7 +5599,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="21" t="s">
         <v>143</v>
       </c>
@@ -5552,7 +5610,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="21" t="s">
         <v>144</v>
       </c>
@@ -5563,7 +5621,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="25" t="s">
         <v>145</v>
       </c>
@@ -5574,7 +5632,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" s="21" t="s">
         <v>146</v>
       </c>
@@ -5585,7 +5643,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" s="27" t="s">
         <v>147</v>
       </c>
@@ -5596,7 +5654,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" s="21" t="s">
         <v>148</v>
       </c>
@@ -5607,7 +5665,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" s="21" t="s">
         <v>149</v>
       </c>
@@ -5618,7 +5676,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" s="38" t="s">
         <v>150</v>
       </c>
@@ -5629,7 +5687,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" s="21" t="s">
         <v>151</v>
       </c>
@@ -5640,7 +5698,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" s="25" t="s">
         <v>152</v>
       </c>
@@ -5651,7 +5709,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" s="27" t="s">
         <v>153</v>
       </c>
@@ -5662,7 +5720,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" s="38" t="s">
         <v>154</v>
       </c>
@@ -5673,7 +5731,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" s="25" t="s">
         <v>155</v>
       </c>
@@ -5684,7 +5742,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A44" s="34" t="s">
         <v>206</v>
       </c>
@@ -5695,7 +5753,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A45" s="34" t="s">
         <v>207</v>
       </c>
@@ -5706,7 +5764,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A46" s="34" t="s">
         <v>208</v>
       </c>
@@ -5717,7 +5775,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="38" t="s">
         <v>220</v>
       </c>
@@ -5728,7 +5786,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" s="38" t="s">
         <v>221</v>
       </c>
@@ -5739,7 +5797,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="38" t="s">
         <v>222</v>
       </c>

</xml_diff>

<commit_message>
US23 - Dhruv Update
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Stevens\Sem 1\CS 555\project 4\CS_555_Project\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EBF635-2011-4345-845B-77DE87963EDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C451A305-E04D-45F2-819B-F892D7DE0A20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="273">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -669,9 +669,6 @@
   </si>
   <si>
     <t>anurag-aman</t>
-  </si>
-  <si>
-    <t>Not Planned</t>
   </si>
   <si>
     <t>Planned</t>
@@ -1537,7 +1534,7 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2527,36 +2524,36 @@
     </row>
     <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="C6" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="D6" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="E6" s="34" t="s">
         <v>204</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="C7" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="D7" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="E7" s="38" t="s">
         <v>218</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2595,8 +2592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:E46"/>
+    <sheetView topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2639,7 +2636,7 @@
         <v>192</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2656,7 +2653,7 @@
         <v>192</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2673,7 +2670,7 @@
         <v>192</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2690,7 +2687,7 @@
         <v>192</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2707,7 +2704,7 @@
         <v>192</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2724,7 +2721,7 @@
         <v>192</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2741,7 +2738,7 @@
         <v>192</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2758,7 +2755,7 @@
         <v>192</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2775,7 +2772,7 @@
         <v>193</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2792,7 +2789,7 @@
         <v>193</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2809,7 +2806,7 @@
         <v>193</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2826,7 +2823,7 @@
         <v>193</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2843,7 +2840,7 @@
         <v>193</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2860,7 +2857,7 @@
         <v>193</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2877,7 +2874,7 @@
         <v>193</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2894,7 +2891,7 @@
         <v>193</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2911,7 +2908,7 @@
         <v>195</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2928,7 +2925,7 @@
         <v>195</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2945,7 +2942,7 @@
         <v>195</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2962,7 +2959,7 @@
         <v>195</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2996,7 +2993,7 @@
         <v>195</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3013,7 +3010,7 @@
         <v>195</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3030,7 +3027,7 @@
         <v>195</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3047,7 +3044,7 @@
         <v>194</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3064,7 +3061,7 @@
         <v>194</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3081,7 +3078,7 @@
         <v>194</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3098,7 +3095,7 @@
         <v>194</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3115,7 +3112,7 @@
         <v>194</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3132,7 +3129,7 @@
         <v>194</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3149,7 +3146,7 @@
         <v>194</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3166,7 +3163,7 @@
         <v>194</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3180,10 +3177,10 @@
         <v>78</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3197,10 +3194,10 @@
         <v>79</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3211,13 +3208,13 @@
         <v>126</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3231,7 +3228,7 @@
         <v>85</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>199</v>
@@ -3245,10 +3242,10 @@
         <v>132</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>199</v>
@@ -3259,16 +3256,16 @@
         <v>1</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3276,27 +3273,30 @@
         <v>1</v>
       </c>
       <c r="B40" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <v>4</v>
+      </c>
+      <c r="B41" s="34" t="s">
         <v>207</v>
       </c>
-      <c r="C40" s="34" t="s">
-        <v>240</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="E40" s="12" t="s">
+      <c r="C41" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>201</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>198</v>
@@ -3313,10 +3313,10 @@
         <v>87</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3330,10 +3330,10 @@
         <v>93</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3347,10 +3347,10 @@
         <v>95</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3364,10 +3364,10 @@
         <v>105</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3381,10 +3381,10 @@
         <v>110</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3392,16 +3392,16 @@
         <v>1</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3409,16 +3409,16 @@
         <v>2</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3426,16 +3426,16 @@
         <v>1</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3652,7 +3652,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3740,7 +3740,7 @@
         <v>30.1</v>
       </c>
       <c r="G4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -3769,10 +3769,10 @@
         <v>42683</v>
       </c>
       <c r="B6" s="12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="12">
         <v>1510</v>
@@ -3818,7 +3818,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3875,7 +3875,7 @@
         <v>192</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E2" s="12">
         <v>50</v>
@@ -3904,7 +3904,7 @@
         <v>192</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E3" s="12">
         <v>50</v>
@@ -3927,13 +3927,13 @@
         <v>144</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>229</v>
-      </c>
       <c r="D4" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E4" s="12">
         <v>50</v>
@@ -3956,13 +3956,13 @@
         <v>130</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>193</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E5" s="12">
         <v>100</v>
@@ -3985,13 +3985,13 @@
         <v>134</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E6" s="12">
         <v>100</v>
@@ -4020,7 +4020,7 @@
         <v>194</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E7" s="12">
         <v>100</v>
@@ -4049,7 +4049,7 @@
         <v>194</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E8" s="12">
         <v>100</v>
@@ -4078,7 +4078,7 @@
         <v>195</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E9" s="12">
         <v>90</v>
@@ -4107,7 +4107,7 @@
         <v>195</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E10" s="12">
         <v>90</v>
@@ -4127,16 +4127,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E11" s="12">
         <v>90</v>
@@ -4156,16 +4156,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E12" s="12">
         <v>90</v>
@@ -4188,13 +4188,13 @@
         <v>126</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E13" s="12">
         <v>100</v>
@@ -4214,16 +4214,16 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E14" s="12">
         <v>100</v>
@@ -4243,16 +4243,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E15" s="12">
         <v>90</v>
@@ -4285,12 +4285,12 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
@@ -4300,7 +4300,7 @@
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -4315,7 +4315,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4363,7 +4363,7 @@
         <v>192</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E2" s="12">
         <v>25</v>
@@ -4392,7 +4392,7 @@
         <v>192</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E3" s="12">
         <v>25</v>
@@ -4421,7 +4421,7 @@
         <v>194</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E4" s="12">
         <v>60</v>
@@ -4450,7 +4450,7 @@
         <v>194</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E5" s="12">
         <v>40</v>
@@ -4473,13 +4473,13 @@
         <v>140</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>195</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E6" s="12">
         <v>60</v>
@@ -4502,13 +4502,13 @@
         <v>129</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>195</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E7" s="12">
         <v>60</v>
@@ -4531,13 +4531,13 @@
         <v>114</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>193</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E8" s="12">
         <v>60</v>
@@ -4560,13 +4560,13 @@
         <v>115</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>193</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E9" s="12">
         <v>60</v>
@@ -4589,13 +4589,13 @@
         <v>133</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E10" s="12">
         <v>60</v>
@@ -4615,16 +4615,16 @@
     </row>
     <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E11" s="12">
         <v>40</v>
@@ -4647,13 +4647,13 @@
         <v>131</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E12" s="12">
         <v>60</v>
@@ -4676,13 +4676,13 @@
         <v>132</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E13" s="12">
         <v>50</v>
@@ -4705,59 +4705,59 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D21" s="52"/>
       <c r="E21" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="52" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D22" s="52"/>
       <c r="E22" s="52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="52" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E25" s="52" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="52" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="52" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -4771,8 +4771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4814,13 +4814,13 @@
         <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>195</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E2" s="12">
         <v>30</v>
@@ -4843,13 +4843,13 @@
         <v>147</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>195</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E3" s="12">
         <v>30</v>
@@ -4878,7 +4878,7 @@
         <v>194</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E4" s="12">
         <v>120</v>
@@ -4907,7 +4907,7 @@
         <v>194</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E5" s="12">
         <v>60</v>
@@ -4936,7 +4936,7 @@
         <v>192</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E6" s="12">
         <v>25</v>
@@ -4965,7 +4965,7 @@
         <v>192</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E7" s="12">
         <v>25</v>
@@ -4994,7 +4994,7 @@
         <v>193</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E8" s="12">
         <v>30</v>
@@ -5023,7 +5023,7 @@
         <v>193</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E9" s="12">
         <v>30</v>
@@ -5049,10 +5049,10 @@
         <v>93</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E10" s="12">
         <v>50</v>
@@ -5078,10 +5078,10 @@
         <v>95</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E11" s="12">
         <v>60</v>
@@ -5104,10 +5104,10 @@
         <v>124</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>199</v>
@@ -5119,7 +5119,7 @@
         <v>60</v>
       </c>
       <c r="G12" s="12">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="H12" s="12">
         <v>60</v>
@@ -5136,7 +5136,7 @@
         <v>79</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>199</v>
@@ -5148,7 +5148,7 @@
         <v>60</v>
       </c>
       <c r="G13" s="12">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="H13" s="12">
         <v>60</v>
@@ -5159,77 +5159,77 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D20" s="52"/>
       <c r="E20" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="52" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D21" s="52"/>
       <c r="E21" s="52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="52" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="52" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E25" s="52" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="52" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="52" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="52" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="52" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -5240,10 +5240,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5293,7 +5293,7 @@
         <v>192</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E2" s="12">
         <v>40</v>
@@ -5313,7 +5313,7 @@
         <v>193</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E3" s="12">
         <v>30</v>
@@ -5333,7 +5333,7 @@
         <v>193</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E4" s="12">
         <v>30</v>
@@ -5353,7 +5353,7 @@
         <v>194</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E5" s="12">
         <v>50</v>
@@ -5373,7 +5373,7 @@
         <v>194</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E6" s="12">
         <v>50</v>
@@ -5393,13 +5393,22 @@
         <v>195</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E7" s="12">
         <v>60</v>
       </c>
       <c r="F7" s="12">
         <v>70</v>
+      </c>
+      <c r="G7" s="12">
+        <v>34</v>
+      </c>
+      <c r="H7" s="12">
+        <v>40</v>
+      </c>
+      <c r="I7" s="50">
+        <v>42697</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -5413,7 +5422,7 @@
         <v>195</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E8" s="12">
         <v>70</v>
@@ -5430,10 +5439,10 @@
         <v>105</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E9" s="12">
         <v>60</v>
@@ -5450,15 +5459,35 @@
         <v>110</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E10" s="12">
         <v>70</v>
       </c>
       <c r="F10" s="12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="12">
+        <v>70</v>
+      </c>
+      <c r="F11" s="12">
         <v>80</v>
       </c>
     </row>
@@ -5472,8 +5501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -5957,68 +5986,68 @@
     </row>
     <row r="44" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A44" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C44" s="45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A45" s="34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C45" s="45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A46" s="34" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B46" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" s="45" t="s">
         <v>213</v>
-      </c>
-      <c r="C46" s="45" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="37" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A48" s="38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 4 Completed - Dhruv
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C451A305-E04D-45F2-819B-F892D7DE0A20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA21F64-0996-446C-8710-3AB8B7B19AF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,12 +401,6 @@
     <t>List upcoming anniversaries</t>
   </si>
   <si>
-    <t>Include input line numbers</t>
-  </si>
-  <si>
-    <t>List line numbers from GEDCOM source file when reporting errors</t>
-  </si>
-  <si>
     <t>Include partial dates</t>
   </si>
   <si>
@@ -894,6 +888,12 @@
   </si>
   <si>
     <t>5. Keep standup calls short and specific to the point</t>
+  </si>
+  <si>
+    <t>List the Individuals who have no Childrens</t>
+  </si>
+  <si>
+    <t>List the names of Individuals who do not have childrens</t>
   </si>
 </sst>
 </file>
@@ -2456,104 +2456,104 @@
     </row>
     <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="34" t="s">
         <v>200</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="D6" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="E6" s="34" t="s">
         <v>202</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="D7" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="E7" s="38" t="s">
         <v>216</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2562,7 +2562,7 @@
         <v>34</v>
       </c>
       <c r="E9" s="54" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F9" s="54"/>
       <c r="G9" s="55"/>
@@ -2593,7 +2593,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2627,16 +2627,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>98</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2644,16 +2644,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>99</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2661,16 +2661,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2678,16 +2678,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>100</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2695,16 +2695,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>102</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2712,16 +2712,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2729,16 +2729,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>104</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2746,16 +2746,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>106</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2763,16 +2763,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2780,16 +2780,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>69</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2797,16 +2797,16 @@
         <v>3</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C12" s="23" t="s">
         <v>68</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2814,16 +2814,16 @@
         <v>3</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>72</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2831,16 +2831,16 @@
         <v>4</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C14" s="23" t="s">
         <v>73</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2848,16 +2848,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C15" s="23" t="s">
         <v>84</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2865,16 +2865,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>88</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2882,16 +2882,16 @@
         <v>4</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>94</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2899,16 +2899,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>70</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2916,16 +2916,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>71</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2933,16 +2933,16 @@
         <v>3</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>82</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2950,16 +2950,16 @@
         <v>2</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>83</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2967,16 +2967,16 @@
         <v>4</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>92</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2984,16 +2984,16 @@
         <v>2</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>96</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3001,16 +3001,16 @@
         <v>3</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3018,16 +3018,16 @@
         <v>4</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>108</v>
+        <v>271</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3035,16 +3035,16 @@
         <v>4</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3052,16 +3052,16 @@
         <v>3</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>75</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3069,16 +3069,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>77</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3086,16 +3086,16 @@
         <v>3</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3103,16 +3103,16 @@
         <v>2</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>91</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3120,16 +3120,16 @@
         <v>2</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C31" s="25" t="s">
         <v>101</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3137,16 +3137,16 @@
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C32" s="25" t="s">
         <v>107</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3154,16 +3154,16 @@
         <v>4</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3171,16 +3171,16 @@
         <v>3</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C34" s="34" t="s">
         <v>78</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3188,16 +3188,16 @@
         <v>3</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C35" s="34" t="s">
         <v>79</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3205,16 +3205,16 @@
         <v>1</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3222,16 +3222,16 @@
         <v>2</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C37" s="34" t="s">
         <v>85</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3239,16 +3239,16 @@
         <v>2</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3256,16 +3256,16 @@
         <v>1</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3273,16 +3273,16 @@
         <v>1</v>
       </c>
       <c r="B40" s="34" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3290,16 +3290,16 @@
         <v>4</v>
       </c>
       <c r="B41" s="34" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3307,16 +3307,16 @@
         <v>2</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C42" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3324,16 +3324,16 @@
         <v>3</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>93</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3341,16 +3341,16 @@
         <v>3</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C44" s="38" t="s">
         <v>95</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3358,16 +3358,16 @@
         <v>4</v>
       </c>
       <c r="B45" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C45" s="38" t="s">
         <v>105</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3375,16 +3375,16 @@
         <v>4</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3392,16 +3392,16 @@
         <v>1</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3409,16 +3409,16 @@
         <v>2</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3426,16 +3426,16 @@
         <v>1</v>
       </c>
       <c r="B49" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="C49" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="C49" s="38" t="s">
-        <v>223</v>
-      </c>
       <c r="D49" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3473,37 +3473,37 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -3526,7 +3526,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B15" s="8">
         <v>41065</v>
@@ -3542,7 +3542,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B16" s="8">
         <v>41078</v>
@@ -3567,7 +3567,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B17" s="8">
         <v>41092</v>
@@ -3592,7 +3592,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B18" s="8">
         <v>41106</v>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B19" s="8">
         <v>41120</v>
@@ -3740,7 +3740,7 @@
         <v>30.1</v>
       </c>
       <c r="G4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -3861,21 +3861,21 @@
         <v>16</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E2" s="12">
         <v>50</v>
@@ -3895,16 +3895,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E3" s="12">
         <v>50</v>
@@ -3924,16 +3924,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E4" s="12">
         <v>50</v>
@@ -3953,16 +3953,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E5" s="12">
         <v>100</v>
@@ -3982,16 +3982,16 @@
     </row>
     <row r="6" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E6" s="12">
         <v>100</v>
@@ -4011,16 +4011,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7" s="33" t="s">
         <v>77</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E7" s="12">
         <v>100</v>
@@ -4040,16 +4040,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>107</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E8" s="12">
         <v>100</v>
@@ -4069,16 +4069,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>70</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E9" s="12">
         <v>90</v>
@@ -4098,16 +4098,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>71</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E10" s="12">
         <v>90</v>
@@ -4127,16 +4127,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E11" s="12">
         <v>90</v>
@@ -4156,16 +4156,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E12" s="12">
         <v>90</v>
@@ -4185,16 +4185,16 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E13" s="12">
         <v>100</v>
@@ -4214,16 +4214,16 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E14" s="12">
         <v>100</v>
@@ -4243,16 +4243,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E15" s="12">
         <v>90</v>
@@ -4285,12 +4285,12 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
@@ -4300,7 +4300,7 @@
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -4354,16 +4354,16 @@
     </row>
     <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E2" s="12">
         <v>25</v>
@@ -4383,16 +4383,16 @@
     </row>
     <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>104</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E3" s="12">
         <v>25</v>
@@ -4412,16 +4412,16 @@
     </row>
     <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>101</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E4" s="12">
         <v>60</v>
@@ -4441,16 +4441,16 @@
     </row>
     <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B5" s="33" t="s">
         <v>91</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E5" s="12">
         <v>40</v>
@@ -4470,16 +4470,16 @@
     </row>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E6" s="12">
         <v>60</v>
@@ -4499,16 +4499,16 @@
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E7" s="12">
         <v>60</v>
@@ -4528,16 +4528,16 @@
     </row>
     <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E8" s="12">
         <v>60</v>
@@ -4557,16 +4557,16 @@
     </row>
     <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E9" s="12">
         <v>60</v>
@@ -4586,16 +4586,16 @@
     </row>
     <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E10" s="12">
         <v>60</v>
@@ -4615,16 +4615,16 @@
     </row>
     <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E11" s="12">
         <v>40</v>
@@ -4644,16 +4644,16 @@
     </row>
     <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E12" s="12">
         <v>60</v>
@@ -4673,16 +4673,16 @@
     </row>
     <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E13" s="12">
         <v>50</v>
@@ -4705,59 +4705,59 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D21" s="52"/>
       <c r="E21" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="52" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D22" s="52"/>
       <c r="E22" s="52" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="52" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="52" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="52" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E25" s="52" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="52" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="52" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -4811,16 +4811,16 @@
     </row>
     <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E2" s="12">
         <v>30</v>
@@ -4840,16 +4840,16 @@
     </row>
     <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E3" s="12">
         <v>30</v>
@@ -4869,16 +4869,16 @@
     </row>
     <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E4" s="12">
         <v>120</v>
@@ -4898,16 +4898,16 @@
     </row>
     <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E5" s="12">
         <v>60</v>
@@ -4927,16 +4927,16 @@
     </row>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>102</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E6" s="12">
         <v>25</v>
@@ -4956,16 +4956,16 @@
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" s="33" t="s">
         <v>106</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E7" s="12">
         <v>25</v>
@@ -4985,16 +4985,16 @@
     </row>
     <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>68</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E8" s="12">
         <v>30</v>
@@ -5014,16 +5014,16 @@
     </row>
     <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>72</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E9" s="12">
         <v>30</v>
@@ -5043,16 +5043,16 @@
     </row>
     <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B10" s="33" t="s">
         <v>93</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E10" s="12">
         <v>50</v>
@@ -5072,16 +5072,16 @@
     </row>
     <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B11" s="33" t="s">
         <v>95</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E11" s="12">
         <v>60</v>
@@ -5101,16 +5101,16 @@
     </row>
     <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E12" s="12">
         <v>60</v>
@@ -5130,16 +5130,16 @@
     </row>
     <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B13" s="33" t="s">
         <v>79</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E13" s="12">
         <v>60</v>
@@ -5159,77 +5159,77 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D20" s="52"/>
       <c r="E20" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="52" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D21" s="52"/>
       <c r="E21" s="52" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="52" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="52" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="52" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="52" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E25" s="52" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="52" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="52" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="52" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="52" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -5243,7 +5243,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5284,16 +5284,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>97</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E2" s="12">
         <v>40</v>
@@ -5304,16 +5304,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>94</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E3" s="12">
         <v>30</v>
@@ -5324,16 +5324,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E4" s="12">
         <v>30</v>
@@ -5344,16 +5344,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E5" s="12">
         <v>50</v>
@@ -5364,16 +5364,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E6" s="12">
         <v>50</v>
@@ -5384,16 +5384,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B7" s="33" t="s">
         <v>92</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E7" s="12">
         <v>60</v>
@@ -5413,16 +5413,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>108</v>
+        <v>271</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E8" s="12">
         <v>70</v>
@@ -5430,19 +5430,28 @@
       <c r="F8" s="12">
         <v>80</v>
       </c>
+      <c r="G8" s="12">
+        <v>18</v>
+      </c>
+      <c r="H8" s="12">
+        <v>15</v>
+      </c>
+      <c r="I8" s="50">
+        <v>42702</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>105</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E9" s="12">
         <v>60</v>
@@ -5453,16 +5462,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E10" s="12">
         <v>70</v>
@@ -5473,16 +5482,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E11" s="12">
         <v>70</v>
@@ -5501,8 +5510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -5513,7 +5522,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>66</v>
@@ -5524,10 +5533,10 @@
     </row>
     <row r="2" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>35</v>
@@ -5535,7 +5544,7 @@
     </row>
     <row r="3" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>69</v>
@@ -5546,7 +5555,7 @@
     </row>
     <row r="4" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>68</v>
@@ -5557,7 +5566,7 @@
     </row>
     <row r="5" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>70</v>
@@ -5568,7 +5577,7 @@
     </row>
     <row r="6" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>71</v>
@@ -5579,7 +5588,7 @@
     </row>
     <row r="7" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>72</v>
@@ -5590,7 +5599,7 @@
     </row>
     <row r="8" spans="1:3" s="31" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>73</v>
@@ -5601,18 +5610,18 @@
     </row>
     <row r="9" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>75</v>
@@ -5623,18 +5632,18 @@
     </row>
     <row r="11" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>77</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>78</v>
@@ -5645,7 +5654,7 @@
     </row>
     <row r="13" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>79</v>
@@ -5656,21 +5665,21 @@
     </row>
     <row r="14" spans="1:3" s="36" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>81</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C15" s="44" t="s">
         <v>42</v>
@@ -5678,7 +5687,7 @@
     </row>
     <row r="16" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>82</v>
@@ -5689,7 +5698,7 @@
     </row>
     <row r="17" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>83</v>
@@ -5700,7 +5709,7 @@
     </row>
     <row r="18" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>84</v>
@@ -5711,7 +5720,7 @@
     </row>
     <row r="19" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>85</v>
@@ -5722,7 +5731,7 @@
     </row>
     <row r="20" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B20" s="34" t="s">
         <v>86</v>
@@ -5733,7 +5742,7 @@
     </row>
     <row r="21" spans="1:3" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>87</v>
@@ -5744,7 +5753,7 @@
     </row>
     <row r="22" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>88</v>
@@ -5755,7 +5764,7 @@
     </row>
     <row r="23" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>91</v>
@@ -5766,7 +5775,7 @@
     </row>
     <row r="24" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>92</v>
@@ -5777,7 +5786,7 @@
     </row>
     <row r="25" spans="1:3" s="37" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>93</v>
@@ -5788,7 +5797,7 @@
     </row>
     <row r="26" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>94</v>
@@ -5799,18 +5808,18 @@
     </row>
     <row r="27" spans="1:3" s="37" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B27" s="38" t="s">
         <v>95</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>96</v>
@@ -5821,18 +5830,18 @@
     </row>
     <row r="29" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>97</v>
       </c>
       <c r="C29" s="47" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B30" s="21" t="s">
         <v>98</v>
@@ -5843,7 +5852,7 @@
     </row>
     <row r="31" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>99</v>
@@ -5854,7 +5863,7 @@
     </row>
     <row r="32" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>100</v>
@@ -5865,7 +5874,7 @@
     </row>
     <row r="33" spans="1:3" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B33" s="25" t="s">
         <v>101</v>
@@ -5876,7 +5885,7 @@
     </row>
     <row r="34" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B34" s="21" t="s">
         <v>102</v>
@@ -5887,10 +5896,10 @@
     </row>
     <row r="35" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C35" s="43" t="s">
         <v>58</v>
@@ -5898,7 +5907,7 @@
     </row>
     <row r="36" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B36" s="21" t="s">
         <v>103</v>
@@ -5909,7 +5918,7 @@
     </row>
     <row r="37" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>104</v>
@@ -5920,7 +5929,7 @@
     </row>
     <row r="38" spans="1:3" s="37" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B38" s="38" t="s">
         <v>105</v>
@@ -5931,7 +5940,7 @@
     </row>
     <row r="39" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B39" s="21" t="s">
         <v>106</v>
@@ -5942,7 +5951,7 @@
     </row>
     <row r="40" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B40" s="25" t="s">
         <v>107</v>
@@ -5951,23 +5960,23 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>108</v>
+        <v>271</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>109</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A42" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C42" s="46" t="s">
         <v>64</v>
@@ -5975,10 +5984,10 @@
     </row>
     <row r="43" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C43" s="44" t="s">
         <v>65</v>
@@ -5986,68 +5995,68 @@
     </row>
     <row r="44" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A44" s="34" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B44" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="C44" s="45" t="s">
         <v>208</v>
-      </c>
-      <c r="C44" s="45" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A45" s="34" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B45" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="C45" s="45" t="s">
         <v>209</v>
-      </c>
-      <c r="C45" s="45" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A46" s="34" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C46" s="45" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B47" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="C47" s="48" t="s">
         <v>222</v>
-      </c>
-      <c r="C47" s="48" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="37" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A48" s="38" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="B49" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="B49" s="38" t="s">
+      <c r="C49" s="48" t="s">
         <v>223</v>
-      </c>
-      <c r="C49" s="48" t="s">
-        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added all the details of sprint 4
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuragaman/Desktop/CS_555_Project-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5624610C-9A16-4843-8EBF-03EEBD51BE3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0137E1DD-18B2-8F4C-B234-B733779DFF9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1344,7 +1344,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1415,7 +1415,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2427,16 +2427,16 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="12" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="12" customWidth="1"/>
+    <col min="4" max="5" width="20.5" style="12" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="21" t="s">
         <v>190</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
         <v>191</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="25" t="s">
         <v>192</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="27" t="s">
         <v>193</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="34" t="s">
         <v>199</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="38" t="s">
         <v>213</v>
       </c>
@@ -2555,8 +2555,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="D9" s="35" t="s">
         <v>34</v>
       </c>
@@ -2591,20 +2591,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:C25"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="6.6328125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>4</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>2</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>3</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>2</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>2</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>3</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
         <v>3</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="12">
         <v>4</v>
       </c>
@@ -2839,10 +2839,10 @@
         <v>191</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="12">
         <v>1</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="12">
         <v>1</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="12">
         <v>4</v>
       </c>
@@ -2890,10 +2890,10 @@
         <v>191</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="12">
         <v>1</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="12">
         <v>1</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="12">
         <v>3</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="12">
         <v>2</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="12">
         <v>4</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="12">
         <v>2</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="12">
         <v>3</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="12">
         <v>4</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="12">
         <v>4</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="12">
         <v>3</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="12">
         <v>1</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="12">
         <v>3</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="12">
         <v>2</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="12">
         <v>2</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="12">
         <v>4</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="12">
         <v>3</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="12">
         <v>3</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="12">
         <v>2</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="12">
         <v>2</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="12">
         <v>1</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="12">
         <v>1</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B41" s="34" t="s">
         <v>206</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="12">
         <v>2</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="12">
         <v>3</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="12">
         <v>3</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="12">
         <v>4</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="12">
         <v>4</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="12">
         <v>1</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="12">
         <v>2</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="12">
         <v>1</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B50" s="39"/>
     </row>
   </sheetData>
@@ -3457,47 +3457,47 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="5"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>159</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -3536,7 +3536,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>161</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>162</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>163</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>164</v>
       </c>
@@ -3651,17 +3651,17 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="16">
         <v>42633</v>
       </c>
@@ -3695,7 +3695,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="16">
         <v>42647</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>30.054446460980031</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="16">
         <v>42654</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="16">
         <v>42668</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>69.697999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="16">
         <v>42683</v>
       </c>
@@ -3770,7 +3770,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="16">
         <v>42708</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="16">
         <v>42728</v>
       </c>
@@ -3806,21 +3806,21 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="11" style="12"/>
-    <col min="5" max="5" width="6.81640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="6.6328125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="12" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>140</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>141</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>142</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>128</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>132</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>121</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>150</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>115</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>116</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>204</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>205</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>124</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>218</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
         <v>220</v>
       </c>
@@ -4255,35 +4255,35 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="13" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="13" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="13" t="s">
         <v>247</v>
       </c>
@@ -4303,12 +4303,12 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>146</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>147</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>143</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>133</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>138</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>127</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>112</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>113</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>131</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>42671</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>219</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>129</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>42672</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>130</v>
       </c>
@@ -4685,15 +4685,15 @@
         <v>42673</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="51"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>256</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="52" t="s">
         <v>252</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="52" t="s">
         <v>253</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="52" t="s">
         <v>254</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="52" t="s">
         <v>257</v>
       </c>
@@ -4735,12 +4735,12 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="52" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="52" t="s">
         <v>263</v>
       </c>
@@ -4757,15 +4757,15 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>126</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>145</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>120</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>125</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
         <v>144</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
         <v>149</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
         <v>114</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
         <v>117</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
         <v>135</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="33" t="s">
         <v>137</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="33" t="s">
         <v>122</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="33" t="s">
         <v>123</v>
       </c>
@@ -5124,12 +5124,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>256</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="52" t="s">
         <v>252</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="52" t="s">
         <v>253</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="52" t="s">
         <v>254</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="52" t="s">
         <v>257</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="52" t="s">
         <v>259</v>
       </c>
@@ -5179,22 +5179,22 @@
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="52" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="52" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="52" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="52" t="s">
         <v>270</v>
       </c>
@@ -5210,17 +5210,17 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="12"/>
     <col min="2" max="2" width="24" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>139</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>136</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>191</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E3" s="12">
         <v>30</v>
@@ -5288,8 +5288,17 @@
       <c r="F3" s="12">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3" s="12">
+        <v>30</v>
+      </c>
+      <c r="H3" s="12">
+        <v>30</v>
+      </c>
+      <c r="I3" s="50">
+        <v>42703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="33" t="s">
         <v>118</v>
       </c>
@@ -5300,7 +5309,7 @@
         <v>191</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E4" s="12">
         <v>30</v>
@@ -5308,8 +5317,17 @@
       <c r="F4" s="12">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="12">
+        <v>25</v>
+      </c>
+      <c r="H4" s="12">
+        <v>35</v>
+      </c>
+      <c r="I4" s="50">
+        <v>42703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>119</v>
       </c>
@@ -5338,7 +5356,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>153</v>
       </c>
@@ -5367,7 +5385,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
         <v>134</v>
       </c>
@@ -5396,7 +5414,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
         <v>151</v>
       </c>
@@ -5425,7 +5443,7 @@
         <v>42702</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
         <v>148</v>
       </c>
@@ -5445,7 +5463,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
         <v>152</v>
       </c>
@@ -5479,13 +5497,13 @@
       <selection activeCell="A41" sqref="A41:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>111</v>
       </c>
@@ -5496,7 +5514,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="23" t="s">
         <v>112</v>
       </c>
@@ -5507,7 +5525,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
         <v>113</v>
       </c>
@@ -5518,7 +5536,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
         <v>114</v>
       </c>
@@ -5529,7 +5547,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" s="27" t="s">
         <v>115</v>
       </c>
@@ -5540,7 +5558,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" s="27" t="s">
         <v>116</v>
       </c>
@@ -5551,7 +5569,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="23" t="s">
         <v>117</v>
       </c>
@@ -5562,7 +5580,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="31" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="31" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" s="23" t="s">
         <v>118</v>
       </c>
@@ -5573,7 +5591,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" s="25" t="s">
         <v>119</v>
       </c>
@@ -5584,7 +5602,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="25" t="s">
         <v>120</v>
       </c>
@@ -5595,7 +5613,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
         <v>121</v>
       </c>
@@ -5606,7 +5624,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="34" t="s">
         <v>122</v>
       </c>
@@ -5617,7 +5635,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" s="34" t="s">
         <v>123</v>
       </c>
@@ -5628,7 +5646,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="36" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="36" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" s="34" t="s">
         <v>124</v>
       </c>
@@ -5639,7 +5657,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
         <v>125</v>
       </c>
@@ -5650,7 +5668,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="27" t="s">
         <v>126</v>
       </c>
@@ -5661,7 +5679,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="27" t="s">
         <v>127</v>
       </c>
@@ -5672,7 +5690,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" s="23" t="s">
         <v>128</v>
       </c>
@@ -5683,7 +5701,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="34" t="s">
         <v>129</v>
       </c>
@@ -5694,7 +5712,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="34" t="s">
         <v>130</v>
       </c>
@@ -5705,7 +5723,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="38" t="s">
         <v>131</v>
       </c>
@@ -5716,7 +5734,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="23" t="s">
         <v>132</v>
       </c>
@@ -5727,7 +5745,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" s="25" t="s">
         <v>133</v>
       </c>
@@ -5738,7 +5756,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" s="27" t="s">
         <v>134</v>
       </c>
@@ -5749,7 +5767,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="37" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="37" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="38" t="s">
         <v>135</v>
       </c>
@@ -5760,7 +5778,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="23" t="s">
         <v>136</v>
       </c>
@@ -5771,7 +5789,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="37" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="37" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A27" s="38" t="s">
         <v>137</v>
       </c>
@@ -5782,7 +5800,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="27" t="s">
         <v>138</v>
       </c>
@@ -5793,7 +5811,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" s="21" t="s">
         <v>139</v>
       </c>
@@ -5804,7 +5822,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="21" t="s">
         <v>140</v>
       </c>
@@ -5815,7 +5833,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="21" t="s">
         <v>141</v>
       </c>
@@ -5826,7 +5844,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="21" t="s">
         <v>142</v>
       </c>
@@ -5837,7 +5855,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="25" t="s">
         <v>143</v>
       </c>
@@ -5848,7 +5866,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" s="21" t="s">
         <v>144</v>
       </c>
@@ -5859,7 +5877,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" s="27" t="s">
         <v>145</v>
       </c>
@@ -5870,7 +5888,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" s="21" t="s">
         <v>146</v>
       </c>
@@ -5881,7 +5899,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" s="21" t="s">
         <v>147</v>
       </c>
@@ -5892,7 +5910,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="37" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" s="38" t="s">
         <v>148</v>
       </c>
@@ -5903,7 +5921,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" s="21" t="s">
         <v>149</v>
       </c>
@@ -5914,7 +5932,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" s="25" t="s">
         <v>150</v>
       </c>
@@ -5925,7 +5943,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" s="27" t="s">
         <v>151</v>
       </c>
@@ -5936,7 +5954,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" s="38" t="s">
         <v>152</v>
       </c>
@@ -5947,7 +5965,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" s="25" t="s">
         <v>153</v>
       </c>
@@ -5958,7 +5976,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A44" s="34" t="s">
         <v>204</v>
       </c>
@@ -5969,7 +5987,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A45" s="34" t="s">
         <v>205</v>
       </c>
@@ -5980,7 +5998,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A46" s="34" t="s">
         <v>206</v>
       </c>
@@ -5991,7 +6009,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="38" t="s">
         <v>218</v>
       </c>
@@ -6002,7 +6020,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="37" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" s="38" t="s">
         <v>219</v>
       </c>
@@ -6013,7 +6031,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="38" t="s">
         <v>220</v>
       </c>

</xml_diff>

<commit_message>
Updated sprint 4 backlog status and burndown chart. Also updated list for keep doing and avoid doing.
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuragaman/Desktop/CS_555_Project-master/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0137E1DD-18B2-8F4C-B234-B733779DFF9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB8F722-5AC2-491A-8DCA-63A9C1B4F3D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="278">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -123,10 +123,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Initials</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Last</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -897,6 +893,21 @@
   </si>
   <si>
     <t>List individual without children</t>
+  </si>
+  <si>
+    <t>Initials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. Fix defects geneated by individuals user story </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. Start documentation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Avoid ambiguous code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Avoid writing unnecessary documentation </t>
   </si>
 </sst>
 </file>
@@ -1344,7 +1355,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1415,7 +1426,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1509,10 +1520,7 @@
                   <c:v>42683</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42708</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42728</c:v>
+                  <c:v>42703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1534,6 +1542,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2427,141 +2441,141 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="12" customWidth="1"/>
     <col min="4" max="5" width="20.5" style="12" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="27" t="s">
+      <c r="E9" s="53" t="s">
         <v>193</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>216</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="53" t="s">
-        <v>194</v>
       </c>
       <c r="F9" s="53"/>
       <c r="G9" s="54"/>
@@ -2591,850 +2605,850 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="6.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>4</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>1</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>3</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>2</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>2</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>3</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>2</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>2</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>3</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <v>3</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
         <v>4</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>1</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <v>1</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <v>4</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>1</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <v>1</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <v>3</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>2</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>4</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>2</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <v>3</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
         <v>4</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <v>4</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <v>3</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
         <v>1</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <v>3</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="12">
         <v>2</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="12">
         <v>2</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="12">
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="12">
         <v>4</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="12">
         <v>3</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="12">
         <v>3</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="12">
         <v>1</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="12">
         <v>2</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="12">
         <v>2</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="12">
         <v>1</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="12">
         <v>1</v>
       </c>
       <c r="B40" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="C40" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="E40" s="12" t="s">
+      <c r="C41" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B41" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>199</v>
-      </c>
       <c r="E41" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="12">
         <v>2</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="12">
         <v>3</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="12">
         <v>3</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="12">
         <v>4</v>
       </c>
       <c r="B45" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="12">
         <v>4</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="12">
         <v>1</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="12">
         <v>2</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="12">
         <v>1</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B50" s="39"/>
     </row>
   </sheetData>
@@ -3453,53 +3467,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="5"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -3511,18 +3525,18 @@
         <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B15" s="8">
         <v>41065</v>
@@ -3536,9 +3550,9 @@
       <c r="F15" s="9"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B16" s="8">
         <v>41078</v>
@@ -3561,9 +3575,9 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" s="8">
         <v>41092</v>
@@ -3586,9 +3600,9 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B18" s="8">
         <v>41106</v>
@@ -3611,9 +3625,9 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B19" s="8">
         <v>41120</v>
@@ -3648,20 +3662,20 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3672,16 +3686,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="16">
         <v>42633</v>
       </c>
@@ -3695,7 +3709,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
         <v>42647</v>
       </c>
@@ -3716,7 +3730,7 @@
         <v>30.054446460980031</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
         <v>42654</v>
       </c>
@@ -3736,10 +3750,10 @@
         <v>30.1</v>
       </c>
       <c r="G4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
         <v>42668</v>
       </c>
@@ -3760,30 +3774,42 @@
         <v>69.697999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
         <v>42683</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B6" s="12">
+        <v>10</v>
+      </c>
+      <c r="C6" s="12">
+        <v>12</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1510</v>
+      </c>
+      <c r="E6" s="12">
+        <v>775</v>
+      </c>
+      <c r="F6" s="17">
+        <v>41.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
-        <v>42708</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
+        <v>42703</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12">
+        <v>10</v>
+      </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="16">
-        <v>42728</v>
-      </c>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -3806,21 +3832,21 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="12" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="12" customWidth="1"/>
     <col min="4" max="4" width="11" style="12"/>
-    <col min="5" max="5" width="6.83203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="12" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -3846,21 +3872,21 @@
         <v>16</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E2" s="12">
         <v>50</v>
@@ -3878,18 +3904,18 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3" s="12">
         <v>50</v>
@@ -3907,18 +3933,18 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>227</v>
-      </c>
       <c r="D4" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E4" s="12">
         <v>50</v>
@@ -3936,18 +3962,18 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5" s="12">
         <v>100</v>
@@ -3965,18 +3991,18 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6" s="12">
         <v>100</v>
@@ -3994,18 +4020,18 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E7" s="12">
         <v>100</v>
@@ -4023,18 +4049,18 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E8" s="12">
         <v>100</v>
@@ -4052,18 +4078,18 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E9" s="12">
         <v>90</v>
@@ -4081,18 +4107,18 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E10" s="12">
         <v>90</v>
@@ -4110,18 +4136,18 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E11" s="12">
         <v>90</v>
@@ -4139,18 +4165,18 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E12" s="12">
         <v>90</v>
@@ -4168,18 +4194,18 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E13" s="12">
         <v>100</v>
@@ -4197,18 +4223,18 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E14" s="12">
         <v>100</v>
@@ -4226,18 +4252,18 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E15" s="12">
         <v>90</v>
@@ -4255,37 +4281,37 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="18"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B17" s="18"/>
-    </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B18" s="18" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B20" s="13" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B19" s="13" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B20" s="13" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="13" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B22" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B23" s="13" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -4303,12 +4329,12 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -4337,18 +4363,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E2" s="12">
         <v>25</v>
@@ -4366,18 +4392,18 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3" s="12">
         <v>25</v>
@@ -4395,18 +4421,18 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E4" s="12">
         <v>60</v>
@@ -4424,18 +4450,18 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5" s="12">
         <v>40</v>
@@ -4453,18 +4479,18 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6" s="12">
         <v>60</v>
@@ -4482,18 +4508,18 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E7" s="12">
         <v>60</v>
@@ -4511,18 +4537,18 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E8" s="12">
         <v>60</v>
@@ -4540,18 +4566,18 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E9" s="12">
         <v>60</v>
@@ -4569,18 +4595,18 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E10" s="12">
         <v>60</v>
@@ -4598,18 +4624,18 @@
         <v>42671</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E11" s="12">
         <v>40</v>
@@ -4627,18 +4653,18 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E12" s="12">
         <v>60</v>
@@ -4656,18 +4682,18 @@
         <v>42672</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E13" s="12">
         <v>50</v>
@@ -4685,64 +4711,64 @@
         <v>42673</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="51"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D21" s="52"/>
       <c r="E21" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="52" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D22" s="52"/>
       <c r="E22" s="52" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="E23" s="52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
+        <v>253</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="E25" s="52" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="52" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="52" t="s">
-        <v>253</v>
-      </c>
-      <c r="E23" s="52" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="52" t="s">
-        <v>254</v>
-      </c>
-      <c r="E24" s="52" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="52" t="s">
-        <v>257</v>
-      </c>
-      <c r="E25" s="52" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="52" t="s">
         <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="52" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="52" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -4757,15 +4783,15 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A19" sqref="A19:I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4794,18 +4820,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E2" s="12">
         <v>30</v>
@@ -4823,18 +4849,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3" s="12">
         <v>30</v>
@@ -4852,18 +4878,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E4" s="12">
         <v>120</v>
@@ -4881,18 +4907,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5" s="12">
         <v>60</v>
@@ -4910,18 +4936,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6" s="12">
         <v>25</v>
@@ -4939,18 +4965,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E7" s="12">
         <v>25</v>
@@ -4968,18 +4994,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E8" s="12">
         <v>30</v>
@@ -4997,18 +5023,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E9" s="12">
         <v>30</v>
@@ -5026,18 +5052,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E10" s="12">
         <v>50</v>
@@ -5055,18 +5081,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="12">
         <v>60</v>
@@ -5084,18 +5110,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E12" s="12">
         <v>60</v>
@@ -5104,18 +5130,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E13" s="12">
         <v>60</v>
@@ -5124,79 +5150,79 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D20" s="52"/>
       <c r="E20" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="52" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D21" s="52"/>
       <c r="E21" s="52" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="E22" s="52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="52" t="s">
+        <v>253</v>
+      </c>
+      <c r="E23" s="52" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="52" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="52" t="s">
-        <v>253</v>
-      </c>
-      <c r="E22" s="52" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="52" t="s">
-        <v>254</v>
-      </c>
-      <c r="E23" s="52" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="52" t="s">
-        <v>257</v>
-      </c>
-      <c r="E24" s="52" t="s">
+      <c r="E25" s="52" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="52" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="52" t="s">
-        <v>259</v>
-      </c>
-      <c r="E25" s="52" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="52" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="52" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="52" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="52" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="52" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="52" t="s">
-        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -5207,20 +5233,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="12"/>
     <col min="2" max="2" width="24" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -5249,15 +5275,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>197</v>
@@ -5268,19 +5294,28 @@
       <c r="F2" s="12">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G2" s="12">
+        <v>26</v>
+      </c>
+      <c r="H2" s="12">
+        <v>90</v>
+      </c>
+      <c r="I2" s="50">
+        <v>42703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3" s="12">
         <v>30</v>
@@ -5298,18 +5333,18 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E4" s="12">
         <v>30</v>
@@ -5327,18 +5362,18 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" s="12">
         <v>50</v>
@@ -5356,18 +5391,18 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6" s="12">
         <v>50</v>
@@ -5385,18 +5420,18 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7" s="12">
         <v>60</v>
@@ -5414,18 +5449,18 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8" s="12">
         <v>40</v>
@@ -5443,18 +5478,18 @@
         <v>42702</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E9" s="12">
         <v>60</v>
@@ -5463,24 +5498,193 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E10" s="12">
         <v>70</v>
       </c>
       <c r="F10" s="12">
         <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="52" t="s">
+        <v>251</v>
+      </c>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52" t="s">
+        <v>257</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18" s="52" t="s">
+        <v>259</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="52" t="s">
+        <v>253</v>
+      </c>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19" s="52" t="s">
+        <v>260</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20" s="52" t="s">
+        <v>261</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="52" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21" s="52" t="s">
+        <v>270</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="52" t="s">
+        <v>262</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22" s="52" t="s">
+        <v>276</v>
+      </c>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="52" t="s">
+        <v>267</v>
+      </c>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
+        <v>268</v>
+      </c>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="52" t="s">
+        <v>269</v>
+      </c>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5493,553 +5697,553 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A41" sqref="A41:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="B2" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A2" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="23" t="s">
+      <c r="C4" s="42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="31" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A4" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A5" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A6" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A7" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="42" t="s">
+      <c r="C9" s="44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="31" customFormat="1" ht="51" x14ac:dyDescent="0.15">
-      <c r="A8" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A9" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A10" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A11" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="44" t="s">
+    <row r="13" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="45" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A12" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="45" t="s">
+    <row r="15" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.15">
-      <c r="A13" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="36" customFormat="1" ht="68" x14ac:dyDescent="0.15">
-      <c r="A14" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" s="34" t="s">
+    <row r="16" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C16" s="43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="37" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="37" customFormat="1" ht="110.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="46" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A15" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A16" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A17" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="31" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A18" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A19" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="45" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A20" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A21" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A22" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A23" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A24" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="37" customFormat="1" ht="51" x14ac:dyDescent="0.15">
-      <c r="A25" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="46" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A26" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="42" t="s">
+    <row r="28" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="43" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="37" customFormat="1" ht="119" x14ac:dyDescent="0.15">
-      <c r="A27" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="B27" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="46" t="s">
+    <row r="29" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="47" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A28" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="43" t="s">
+    <row r="30" spans="1:3" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="47" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A29" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="47" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A30" s="21" t="s">
+    <row r="31" spans="1:3" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B31" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C31" s="47" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="29" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A31" s="21" t="s">
+    <row r="32" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B32" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C32" s="47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A32" s="21" t="s">
+    <row r="33" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B33" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C33" s="44" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A33" s="25" t="s">
+    <row r="34" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B34" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C34" s="47" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A34" s="21" t="s">
+    <row r="35" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B35" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A35" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="43" t="s">
+      <c r="C36" s="47" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A36" s="21" t="s">
+    <row r="37" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B37" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C37" s="47" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A37" s="21" t="s">
+    <row r="38" spans="1:3" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B38" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="47" t="s">
+      <c r="C38" s="46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A38" s="38" t="s">
+    <row r="39" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B39" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="46" t="s">
+      <c r="C39" s="47" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A39" s="21" t="s">
+    <row r="40" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B40" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="47" t="s">
+      <c r="C40" s="44" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A40" s="25" t="s">
+    <row r="41" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B41" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="44" t="s">
+      <c r="C42" s="46" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A41" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="B41" s="27" t="s">
-        <v>273</v>
-      </c>
-      <c r="C41" s="43" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="37" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A42" s="38" t="s">
+    <row r="43" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A43" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="B42" s="38" t="s">
+      <c r="B43" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="46" t="s">
+      <c r="C43" s="44" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A43" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="44" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A44" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="C44" s="45" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B45" s="34" t="s">
         <v>207</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C45" s="45" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A45" s="34" t="s">
+    <row r="46" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="B45" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="C45" s="45" t="s">
+      <c r="B46" s="34" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A46" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="B46" s="34" t="s">
+      <c r="C46" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="C46" s="45" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="47" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="C47" s="48" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A48" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="B47" s="38" t="s">
+      <c r="B48" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="B49" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="C47" s="48" t="s">
+      <c r="C49" s="48" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A48" s="38" t="s">
-        <v>219</v>
-      </c>
-      <c r="B48" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="C48" s="48" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A49" s="38" t="s">
-        <v>220</v>
-      </c>
-      <c r="B49" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="C49" s="48" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User story 41 Completed
Updated xls
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Stevens\Sem 1\CS 555\project 4\CS_555_Project\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB8F722-5AC2-491A-8DCA-63A9C1B4F3D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA22972-1C5C-4DEB-A1F8-9572628A365F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="960" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2437,7 +2437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -2605,8 +2605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3377,7 +3377,7 @@
         <v>212</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -3394,7 +3394,7 @@
         <v>212</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -3467,7 +3467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -4783,7 +4783,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:I29"/>
+      <selection activeCell="D9" sqref="D9:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5063,7 +5063,7 @@
         <v>212</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E10" s="12">
         <v>50</v>
@@ -5092,7 +5092,7 @@
         <v>212</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E11" s="12">
         <v>60</v>
@@ -5236,7 +5236,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5488,14 +5488,23 @@
       <c r="C9" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>196</v>
+      <c r="D9" s="12" t="s">
+        <v>197</v>
       </c>
       <c r="E9" s="12">
         <v>60</v>
       </c>
       <c r="F9" s="12">
         <v>70</v>
+      </c>
+      <c r="G9" s="12">
+        <v>41</v>
+      </c>
+      <c r="H9" s="12">
+        <v>35</v>
+      </c>
+      <c r="I9" s="50">
+        <v>42703</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -5508,14 +5517,23 @@
       <c r="C10" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="D10" s="33" t="s">
-        <v>196</v>
+      <c r="D10" s="12" t="s">
+        <v>197</v>
       </c>
       <c r="E10" s="12">
         <v>70</v>
       </c>
       <c r="F10" s="12">
         <v>80</v>
+      </c>
+      <c r="G10" s="12">
+        <v>51</v>
+      </c>
+      <c r="H10" s="12">
+        <v>20</v>
+      </c>
+      <c r="I10" s="50">
+        <v>42703</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -5697,8 +5715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:B41"/>
+    <sheetView topLeftCell="A36" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Excel Update - BurnDown
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiNeilPradeepReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Stevens\Sem 1\CS 555\project 4\CS_555_Project\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA22972-1C5C-4DEB-A1F8-9572628A365F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B198BE53-719E-4C7E-9927-B316D436E7AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="960" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="277">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -659,9 +659,6 @@
   </si>
   <si>
     <t>anurag-aman</t>
-  </si>
-  <si>
-    <t>Not Planned</t>
   </si>
   <si>
     <t>Planned</t>
@@ -1155,7 +1152,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1241,6 +1238,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2437,22 +2435,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="12" customWidth="1"/>
-    <col min="4" max="5" width="20.5" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="12" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" style="12" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>20</v>
@@ -2467,7 +2465,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>189</v>
       </c>
@@ -2484,7 +2482,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>190</v>
       </c>
@@ -2501,7 +2499,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>191</v>
       </c>
@@ -2518,7 +2516,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>192</v>
       </c>
@@ -2535,42 +2533,42 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="C6" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="D6" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="E6" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="E6" s="34" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="C7" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="D7" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="E7" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="E7" s="38" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="35" t="s">
         <v>33</v>
       </c>
@@ -2606,19 +2604,19 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E46"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.6328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>28</v>
       </c>
@@ -2635,7 +2633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2649,10 +2647,10 @@
         <v>189</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -2666,10 +2664,10 @@
         <v>189</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>4</v>
       </c>
@@ -2683,10 +2681,10 @@
         <v>189</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -2700,10 +2698,10 @@
         <v>189</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -2717,10 +2715,10 @@
         <v>189</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -2734,10 +2732,10 @@
         <v>189</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>2</v>
       </c>
@@ -2751,10 +2749,10 @@
         <v>189</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>3</v>
       </c>
@@ -2768,10 +2766,10 @@
         <v>189</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>2</v>
       </c>
@@ -2785,10 +2783,10 @@
         <v>190</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>2</v>
       </c>
@@ -2802,10 +2800,10 @@
         <v>190</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>3</v>
       </c>
@@ -2819,10 +2817,10 @@
         <v>190</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>3</v>
       </c>
@@ -2836,10 +2834,10 @@
         <v>190</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>4</v>
       </c>
@@ -2853,10 +2851,10 @@
         <v>190</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>1</v>
       </c>
@@ -2870,10 +2868,10 @@
         <v>190</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>1</v>
       </c>
@@ -2887,10 +2885,10 @@
         <v>190</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>4</v>
       </c>
@@ -2904,10 +2902,10 @@
         <v>190</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>1</v>
       </c>
@@ -2921,10 +2919,10 @@
         <v>192</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>1</v>
       </c>
@@ -2938,10 +2936,10 @@
         <v>192</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>3</v>
       </c>
@@ -2955,10 +2953,10 @@
         <v>192</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>2</v>
       </c>
@@ -2972,10 +2970,10 @@
         <v>192</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>4</v>
       </c>
@@ -2989,10 +2987,10 @@
         <v>192</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>2</v>
       </c>
@@ -3006,10 +3004,10 @@
         <v>192</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>3</v>
       </c>
@@ -3023,10 +3021,10 @@
         <v>192</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>4</v>
       </c>
@@ -3034,16 +3032,16 @@
         <v>150</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>192</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>4</v>
       </c>
@@ -3057,10 +3055,10 @@
         <v>191</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>3</v>
       </c>
@@ -3074,10 +3072,10 @@
         <v>191</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>1</v>
       </c>
@@ -3091,10 +3089,10 @@
         <v>191</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>3</v>
       </c>
@@ -3108,10 +3106,10 @@
         <v>191</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>2</v>
       </c>
@@ -3125,10 +3123,10 @@
         <v>191</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>2</v>
       </c>
@@ -3142,10 +3140,10 @@
         <v>191</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -3159,10 +3157,10 @@
         <v>191</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>4</v>
       </c>
@@ -3176,10 +3174,10 @@
         <v>191</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>3</v>
       </c>
@@ -3190,13 +3188,13 @@
         <v>77</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>3</v>
       </c>
@@ -3207,13 +3205,13 @@
         <v>78</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -3221,16 +3219,16 @@
         <v>123</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>2</v>
       </c>
@@ -3241,13 +3239,13 @@
         <v>84</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>2</v>
       </c>
@@ -3255,64 +3253,67 @@
         <v>129</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>1</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>1</v>
       </c>
       <c r="B40" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <v>4</v>
+      </c>
+      <c r="B41" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="C40" s="34" t="s">
-        <v>237</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E40" s="12" t="s">
+      <c r="C41" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>198</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>2</v>
       </c>
@@ -3323,13 +3324,13 @@
         <v>86</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>3</v>
       </c>
@@ -3340,13 +3341,13 @@
         <v>92</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>3</v>
       </c>
@@ -3357,13 +3358,13 @@
         <v>94</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>4</v>
       </c>
@@ -3374,13 +3375,13 @@
         <v>104</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>4</v>
       </c>
@@ -3391,64 +3392,64 @@
         <v>107</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>1</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>2</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>1</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" s="39"/>
     </row>
   </sheetData>
@@ -3468,17 +3469,17 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="5"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="5"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3661,21 +3662,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3695,7 +3696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>42633</v>
       </c>
@@ -3709,7 +3710,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>42647</v>
       </c>
@@ -3730,7 +3731,7 @@
         <v>30.054446460980031</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>42654</v>
       </c>
@@ -3750,10 +3751,10 @@
         <v>30.1</v>
       </c>
       <c r="G4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>42668</v>
       </c>
@@ -3774,7 +3775,7 @@
         <v>69.697999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>42683</v>
       </c>
@@ -3794,7 +3795,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>42703</v>
       </c>
@@ -3804,11 +3805,18 @@
       <c r="C7" s="12">
         <v>10</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D7" s="12">
+        <v>1854</v>
+      </c>
+      <c r="E7" s="12">
+        <v>320</v>
+      </c>
+      <c r="F7" s="17">
+        <f>(D7-D6)/E7*60</f>
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -3832,21 +3840,21 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="27.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" style="12" customWidth="1"/>
     <col min="4" max="4" width="11" style="12"/>
-    <col min="5" max="5" width="6.875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="6.625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="6.6328125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.6328125" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -3875,7 +3883,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>139</v>
       </c>
@@ -3886,7 +3894,7 @@
         <v>189</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E2" s="12">
         <v>50</v>
@@ -3904,7 +3912,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>140</v>
       </c>
@@ -3915,7 +3923,7 @@
         <v>189</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E3" s="12">
         <v>50</v>
@@ -3933,18 +3941,18 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>141</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>226</v>
-      </c>
       <c r="D4" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="12">
         <v>50</v>
@@ -3962,18 +3970,18 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>127</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>190</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" s="12">
         <v>100</v>
@@ -3991,18 +3999,18 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>131</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6" s="12">
         <v>100</v>
@@ -4020,7 +4028,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>120</v>
       </c>
@@ -4031,7 +4039,7 @@
         <v>191</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7" s="12">
         <v>100</v>
@@ -4049,7 +4057,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>149</v>
       </c>
@@ -4060,7 +4068,7 @@
         <v>191</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8" s="12">
         <v>100</v>
@@ -4078,7 +4086,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>114</v>
       </c>
@@ -4089,7 +4097,7 @@
         <v>192</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E9" s="12">
         <v>90</v>
@@ -4107,7 +4115,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>115</v>
       </c>
@@ -4118,7 +4126,7 @@
         <v>192</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E10" s="12">
         <v>90</v>
@@ -4136,18 +4144,18 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="12">
         <v>90</v>
@@ -4165,18 +4173,18 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E12" s="12">
         <v>90</v>
@@ -4194,18 +4202,18 @@
         <v>42647</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>123</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E13" s="12">
         <v>100</v>
@@ -4223,18 +4231,18 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E14" s="12">
         <v>100</v>
@@ -4252,18 +4260,18 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E15" s="12">
         <v>90</v>
@@ -4281,37 +4289,37 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B20" s="13" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -4329,12 +4337,12 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -4363,7 +4371,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>145</v>
       </c>
@@ -4374,7 +4382,7 @@
         <v>189</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E2" s="12">
         <v>25</v>
@@ -4392,7 +4400,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>146</v>
       </c>
@@ -4403,7 +4411,7 @@
         <v>189</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E3" s="12">
         <v>25</v>
@@ -4421,7 +4429,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>142</v>
       </c>
@@ -4432,7 +4440,7 @@
         <v>191</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="12">
         <v>60</v>
@@ -4450,7 +4458,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>132</v>
       </c>
@@ -4461,7 +4469,7 @@
         <v>191</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" s="12">
         <v>40</v>
@@ -4479,18 +4487,18 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>137</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>192</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6" s="12">
         <v>60</v>
@@ -4508,18 +4516,18 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>126</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>192</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7" s="12">
         <v>60</v>
@@ -4537,18 +4545,18 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>111</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>190</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8" s="12">
         <v>60</v>
@@ -4566,18 +4574,18 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>112</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>190</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E9" s="12">
         <v>60</v>
@@ -4595,18 +4603,18 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>130</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E10" s="12">
         <v>60</v>
@@ -4624,18 +4632,18 @@
         <v>42671</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="12">
         <v>40</v>
@@ -4653,18 +4661,18 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>128</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E12" s="12">
         <v>60</v>
@@ -4682,18 +4690,18 @@
         <v>42672</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>129</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E13" s="12">
         <v>50</v>
@@ -4711,64 +4719,64 @@
         <v>42673</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="51"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D21" s="52"/>
       <c r="E21" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="52" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D22" s="52"/>
       <c r="E22" s="52" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="52" t="s">
+        <v>251</v>
+      </c>
+      <c r="E23" s="52" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="52" t="s">
+        <v>255</v>
+      </c>
+      <c r="E25" s="52" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="52" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="52" t="s">
-        <v>252</v>
-      </c>
-      <c r="E23" s="52" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="52" t="s">
-        <v>253</v>
-      </c>
-      <c r="E24" s="52" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="E25" s="52" t="s">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="52" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="52" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="52" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -4783,15 +4791,15 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4820,18 +4828,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>125</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>192</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E2" s="12">
         <v>30</v>
@@ -4849,18 +4857,18 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>144</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>192</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E3" s="12">
         <v>30</v>
@@ -4878,7 +4886,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>119</v>
       </c>
@@ -4889,7 +4897,7 @@
         <v>191</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="12">
         <v>120</v>
@@ -4907,7 +4915,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>124</v>
       </c>
@@ -4918,7 +4926,7 @@
         <v>191</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" s="12">
         <v>60</v>
@@ -4936,7 +4944,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>143</v>
       </c>
@@ -4947,7 +4955,7 @@
         <v>189</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6" s="12">
         <v>25</v>
@@ -4965,7 +4973,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>148</v>
       </c>
@@ -4976,7 +4984,7 @@
         <v>189</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7" s="12">
         <v>25</v>
@@ -4994,7 +5002,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>113</v>
       </c>
@@ -5005,7 +5013,7 @@
         <v>190</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8" s="12">
         <v>30</v>
@@ -5023,7 +5031,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>116</v>
       </c>
@@ -5034,7 +5042,7 @@
         <v>190</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E9" s="12">
         <v>30</v>
@@ -5052,7 +5060,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>134</v>
       </c>
@@ -5060,10 +5068,10 @@
         <v>92</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E10" s="12">
         <v>50</v>
@@ -5081,7 +5089,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>136</v>
       </c>
@@ -5089,10 +5097,10 @@
         <v>94</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="12">
         <v>60</v>
@@ -5110,15 +5118,15 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>121</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>196</v>
@@ -5129,8 +5137,17 @@
       <c r="F12" s="12">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G12" s="12">
+        <v>29</v>
+      </c>
+      <c r="H12" s="12">
+        <v>50</v>
+      </c>
+      <c r="I12" s="55">
+        <v>42683</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>122</v>
       </c>
@@ -5138,7 +5155,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>196</v>
@@ -5149,80 +5166,89 @@
       <c r="F13" s="12">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G13" s="12">
+        <v>25</v>
+      </c>
+      <c r="H13" s="12">
+        <v>50</v>
+      </c>
+      <c r="I13" s="55">
+        <v>42683</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D20" s="52"/>
       <c r="E20" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="52" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D21" s="52"/>
       <c r="E21" s="52" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="52" t="s">
+        <v>251</v>
+      </c>
+      <c r="E22" s="52" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="E23" s="52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
+        <v>255</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="52" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="52" t="s">
-        <v>252</v>
-      </c>
-      <c r="E22" s="52" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="52" t="s">
-        <v>253</v>
-      </c>
-      <c r="E23" s="52" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="E24" s="52" t="s">
+      <c r="E25" s="52" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="52" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="52" t="s">
-        <v>258</v>
-      </c>
-      <c r="E25" s="52" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="52" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="52" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="52" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="52" t="s">
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="52" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="52" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -5239,14 +5265,14 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="12"/>
     <col min="2" max="2" width="24" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -5275,7 +5301,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>138</v>
       </c>
@@ -5286,7 +5312,7 @@
         <v>189</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E2" s="12">
         <v>40</v>
@@ -5304,7 +5330,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>135</v>
       </c>
@@ -5315,7 +5341,7 @@
         <v>190</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E3" s="12">
         <v>30</v>
@@ -5333,7 +5359,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>117</v>
       </c>
@@ -5344,7 +5370,7 @@
         <v>190</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="12">
         <v>30</v>
@@ -5362,7 +5388,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>118</v>
       </c>
@@ -5373,7 +5399,7 @@
         <v>191</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E5" s="12">
         <v>50</v>
@@ -5391,7 +5417,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>152</v>
       </c>
@@ -5402,7 +5428,7 @@
         <v>191</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E6" s="12">
         <v>50</v>
@@ -5420,7 +5446,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>133</v>
       </c>
@@ -5431,7 +5457,7 @@
         <v>192</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E7" s="12">
         <v>60</v>
@@ -5449,18 +5475,18 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>150</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>192</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E8" s="12">
         <v>40</v>
@@ -5478,7 +5504,7 @@
         <v>42702</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>147</v>
       </c>
@@ -5486,10 +5512,10 @@
         <v>104</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E9" s="12">
         <v>60</v>
@@ -5507,7 +5533,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>151</v>
       </c>
@@ -5515,10 +5541,10 @@
         <v>107</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E10" s="12">
         <v>70</v>
@@ -5536,9 +5562,9 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -5549,129 +5575,129 @@
       <c r="H15"/>
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16" s="52"/>
       <c r="E16" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17" s="52"/>
       <c r="E17" s="52" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" s="52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" s="52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" s="52" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" s="52" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22" s="52" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -5682,9 +5708,9 @@
       <c r="H24"/>
       <c r="I24"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -5695,14 +5721,14 @@
       <c r="H25"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5719,13 +5745,13 @@
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>110</v>
       </c>
@@ -5736,7 +5762,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>111</v>
       </c>
@@ -5747,7 +5773,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>112</v>
       </c>
@@ -5758,7 +5784,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>113</v>
       </c>
@@ -5769,7 +5795,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>114</v>
       </c>
@@ -5780,7 +5806,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>115</v>
       </c>
@@ -5791,7 +5817,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>116</v>
       </c>
@@ -5802,7 +5828,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="31" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="31" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>117</v>
       </c>
@@ -5813,7 +5839,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>118</v>
       </c>
@@ -5824,7 +5850,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>119</v>
       </c>
@@ -5835,7 +5861,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>120</v>
       </c>
@@ -5846,7 +5872,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>121</v>
       </c>
@@ -5857,7 +5883,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>122</v>
       </c>
@@ -5868,7 +5894,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="36" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>123</v>
       </c>
@@ -5879,7 +5905,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>124</v>
       </c>
@@ -5890,7 +5916,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>125</v>
       </c>
@@ -5901,7 +5927,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>126</v>
       </c>
@@ -5912,7 +5938,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>127</v>
       </c>
@@ -5923,7 +5949,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>128</v>
       </c>
@@ -5934,7 +5960,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>129</v>
       </c>
@@ -5945,7 +5971,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>130</v>
       </c>
@@ -5956,7 +5982,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>131</v>
       </c>
@@ -5967,7 +5993,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>132</v>
       </c>
@@ -5978,7 +6004,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>133</v>
       </c>
@@ -5989,7 +6015,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="37" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="37" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
         <v>134</v>
       </c>
@@ -6000,7 +6026,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="31" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>135</v>
       </c>
@@ -6011,7 +6037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="37" customFormat="1" ht="110.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="37" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
         <v>136</v>
       </c>
@@ -6022,7 +6048,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>137</v>
       </c>
@@ -6033,7 +6059,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>138</v>
       </c>
@@ -6044,7 +6070,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>139</v>
       </c>
@@ -6055,7 +6081,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>140</v>
       </c>
@@ -6066,7 +6092,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>141</v>
       </c>
@@ -6077,7 +6103,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>142</v>
       </c>
@@ -6088,7 +6114,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>143</v>
       </c>
@@ -6099,7 +6125,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>144</v>
       </c>
@@ -6110,7 +6136,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>145</v>
       </c>
@@ -6121,7 +6147,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>146</v>
       </c>
@@ -6132,7 +6158,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="37" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
         <v>147</v>
       </c>
@@ -6143,7 +6169,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>148</v>
       </c>
@@ -6154,7 +6180,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>149</v>
       </c>
@@ -6165,18 +6191,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>150</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A42" s="38" t="s">
         <v>151</v>
       </c>
@@ -6187,7 +6213,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="32" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>152</v>
       </c>
@@ -6198,70 +6224,70 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A44" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="C44" s="45" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="36" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B45" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C45" s="45" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="34" t="s">
+    <row r="46" spans="1:3" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A46" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="B45" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="C45" s="45" t="s">
+      <c r="B46" s="34" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="B46" s="34" t="s">
+      <c r="C46" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="C46" s="45" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="B47" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="C47" s="48" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="37" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A48" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="B47" s="38" t="s">
+      <c r="B48" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="37" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A49" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="B49" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="C47" s="48" t="s">
+      <c r="C49" s="48" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="38" t="s">
-        <v>218</v>
-      </c>
-      <c r="B48" s="38" t="s">
-        <v>224</v>
-      </c>
-      <c r="C48" s="48" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="38" t="s">
-        <v>219</v>
-      </c>
-      <c r="B49" s="38" t="s">
-        <v>221</v>
-      </c>
-      <c r="C49" s="48" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>